<commit_message>
fixed bye week matchup id error, added new matchups and playerpoints to BI file, fixed resultant errors
</commit_message>
<xml_diff>
--- a/matchups.xlsx
+++ b/matchups.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K217"/>
+  <dimension ref="A1:O217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Projected_score</t>
+          <t>Projected Points</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Actual_score</t>
+          <t>Actual Points</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -481,12 +481,32 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>matchup_header</t>
+          <t>Matchup Header</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>result</t>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Number</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>MatchupKey</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>WeeklyMatchupID</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
         </is>
       </c>
     </row>
@@ -536,6 +556,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -583,6 +617,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -630,6 +678,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>1Sith Happens</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -677,6 +739,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>1Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -724,6 +800,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>1Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -771,6 +861,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>3</v>
+      </c>
+      <c r="O7" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -818,6 +922,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L8" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>1Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>4</v>
+      </c>
+      <c r="O8" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -865,6 +983,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>1Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>4</v>
+      </c>
+      <c r="O9" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -912,6 +1044,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L10" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>1Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>5</v>
+      </c>
+      <c r="O10" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -959,6 +1105,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>1Apex Predators</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>5</v>
+      </c>
+      <c r="O11" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1006,6 +1166,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L12" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>1Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>6</v>
+      </c>
+      <c r="O12" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1053,6 +1227,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>1Bring the heat</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O13" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1100,6 +1288,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L14" t="n">
+        <v>2</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>2Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1147,6 +1349,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1194,6 +1410,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L16" t="n">
+        <v>2</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>2</v>
+      </c>
+      <c r="O16" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1241,6 +1471,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>2Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>2</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1288,6 +1532,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L18" t="n">
+        <v>2</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>3</v>
+      </c>
+      <c r="O18" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1335,6 +1593,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2Sith Happens</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>3</v>
+      </c>
+      <c r="O19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1382,6 +1654,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L20" t="n">
+        <v>2</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>4</v>
+      </c>
+      <c r="O20" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1429,6 +1715,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2Apex Predators</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>4</v>
+      </c>
+      <c r="O21" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1476,6 +1776,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L22" t="n">
+        <v>2</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>2Bring the heat</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>5</v>
+      </c>
+      <c r="O22" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1523,6 +1837,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>5</v>
+      </c>
+      <c r="O23" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1570,6 +1898,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L24" t="n">
+        <v>2</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>2Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>6</v>
+      </c>
+      <c r="O24" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1617,6 +1959,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>2Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>6</v>
+      </c>
+      <c r="O25" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1664,6 +2020,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L26" t="n">
+        <v>2</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>3Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1711,6 +2081,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>3Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1758,6 +2142,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L28" t="n">
+        <v>2</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>3Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>2</v>
+      </c>
+      <c r="O28" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1805,6 +2203,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>3Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>2</v>
+      </c>
+      <c r="O29" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1852,6 +2264,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L30" t="n">
+        <v>2</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>3Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>3</v>
+      </c>
+      <c r="O30" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1899,6 +2325,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L31" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>3Sith Happens</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>3</v>
+      </c>
+      <c r="O31" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1946,6 +2386,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L32" t="n">
+        <v>2</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>3Bring the heat</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>4</v>
+      </c>
+      <c r="O32" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1993,6 +2447,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L33" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>3Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>4</v>
+      </c>
+      <c r="O33" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2040,6 +2508,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L34" t="n">
+        <v>2</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>3Apex Predators</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>5</v>
+      </c>
+      <c r="O34" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2087,6 +2569,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>3Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>5</v>
+      </c>
+      <c r="O35" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2134,6 +2630,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L36" t="n">
+        <v>2</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>3Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>6</v>
+      </c>
+      <c r="O36" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2181,6 +2691,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L37" t="n">
+        <v>1</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>3Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>6</v>
+      </c>
+      <c r="O37" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2228,6 +2752,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L38" t="n">
+        <v>2</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>4Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2275,6 +2813,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>4Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2322,6 +2874,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L40" t="n">
+        <v>2</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>4Sith Happens</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>2</v>
+      </c>
+      <c r="O40" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2369,6 +2935,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L41" t="n">
+        <v>1</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>4Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>2</v>
+      </c>
+      <c r="O41" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2416,6 +2996,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L42" t="n">
+        <v>2</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>4Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>3</v>
+      </c>
+      <c r="O42" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2463,6 +3057,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L43" t="n">
+        <v>1</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>4Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>3</v>
+      </c>
+      <c r="O43" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2510,6 +3118,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L44" t="n">
+        <v>2</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>4Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N44" t="n">
+        <v>4</v>
+      </c>
+      <c r="O44" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2557,6 +3179,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L45" t="n">
+        <v>1</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>4Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N45" t="n">
+        <v>4</v>
+      </c>
+      <c r="O45" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2604,6 +3240,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L46" t="n">
+        <v>2</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>4Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N46" t="n">
+        <v>5</v>
+      </c>
+      <c r="O46" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2651,6 +3301,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L47" t="n">
+        <v>1</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>4Bring the heat</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>5</v>
+      </c>
+      <c r="O47" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2698,6 +3362,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L48" t="n">
+        <v>2</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>4Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>6</v>
+      </c>
+      <c r="O48" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2745,6 +3423,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L49" t="n">
+        <v>1</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>4Apex Predators</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>6</v>
+      </c>
+      <c r="O49" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2792,6 +3484,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L50" t="n">
+        <v>2</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>5Sith Happens</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>1</v>
+      </c>
+      <c r="O50" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2839,6 +3545,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L51" t="n">
+        <v>1</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>5Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>1</v>
+      </c>
+      <c r="O51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2886,6 +3606,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L52" t="n">
+        <v>2</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>5Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>2</v>
+      </c>
+      <c r="O52" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2933,6 +3667,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L53" t="n">
+        <v>1</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>5Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>2</v>
+      </c>
+      <c r="O53" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2980,6 +3728,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L54" t="n">
+        <v>2</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>5Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N54" t="n">
+        <v>3</v>
+      </c>
+      <c r="O54" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3027,6 +3789,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L55" t="n">
+        <v>1</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>5Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N55" t="n">
+        <v>3</v>
+      </c>
+      <c r="O55" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3074,6 +3850,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L56" t="n">
+        <v>2</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>5Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N56" t="n">
+        <v>4</v>
+      </c>
+      <c r="O56" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3121,6 +3911,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L57" t="n">
+        <v>1</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>5Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>4</v>
+      </c>
+      <c r="O57" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3168,6 +3972,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L58" t="n">
+        <v>2</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>5Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N58" t="n">
+        <v>5</v>
+      </c>
+      <c r="O58" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3215,6 +4033,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L59" t="n">
+        <v>1</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>5Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>5</v>
+      </c>
+      <c r="O59" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3262,6 +4094,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L60" t="n">
+        <v>2</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>5Bring the heat</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>6</v>
+      </c>
+      <c r="O60" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3309,6 +4155,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L61" t="n">
+        <v>1</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>5Apex Predators</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>6</v>
+      </c>
+      <c r="O61" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3356,6 +4216,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L62" t="n">
+        <v>2</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>6Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>1</v>
+      </c>
+      <c r="O62" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3403,6 +4277,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L63" t="n">
+        <v>1</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>6Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>1</v>
+      </c>
+      <c r="O63" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3450,6 +4338,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L64" t="n">
+        <v>2</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>6Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>2</v>
+      </c>
+      <c r="O64" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3497,6 +4399,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L65" t="n">
+        <v>1</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>6Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>2</v>
+      </c>
+      <c r="O65" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3544,6 +4460,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L66" t="n">
+        <v>2</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>6Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>3</v>
+      </c>
+      <c r="O66" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3591,6 +4521,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L67" t="n">
+        <v>1</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>6Apex Predators</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>3</v>
+      </c>
+      <c r="O67" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3638,6 +4582,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L68" t="n">
+        <v>2</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>6Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N68" t="n">
+        <v>4</v>
+      </c>
+      <c r="O68" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3685,6 +4643,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L69" t="n">
+        <v>1</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>6Bring the heat</t>
+        </is>
+      </c>
+      <c r="N69" t="n">
+        <v>4</v>
+      </c>
+      <c r="O69" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3732,6 +4704,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L70" t="n">
+        <v>2</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>6Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N70" t="n">
+        <v>5</v>
+      </c>
+      <c r="O70" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3779,6 +4765,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L71" t="n">
+        <v>1</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>6Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>5</v>
+      </c>
+      <c r="O71" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3826,6 +4826,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L72" t="n">
+        <v>2</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>6Sith Happens</t>
+        </is>
+      </c>
+      <c r="N72" t="n">
+        <v>6</v>
+      </c>
+      <c r="O72" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3873,6 +4887,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L73" t="n">
+        <v>1</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>6Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N73" t="n">
+        <v>6</v>
+      </c>
+      <c r="O73" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3920,6 +4948,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L74" t="n">
+        <v>2</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>7Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v>1</v>
+      </c>
+      <c r="O74" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3967,6 +5009,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L75" t="n">
+        <v>1</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>7Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v>1</v>
+      </c>
+      <c r="O75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4014,6 +5070,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L76" t="n">
+        <v>2</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>7Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N76" t="n">
+        <v>2</v>
+      </c>
+      <c r="O76" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4061,6 +5131,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L77" t="n">
+        <v>1</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>7Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N77" t="n">
+        <v>2</v>
+      </c>
+      <c r="O77" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4108,6 +5192,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L78" t="n">
+        <v>2</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>7Apex Predators</t>
+        </is>
+      </c>
+      <c r="N78" t="n">
+        <v>3</v>
+      </c>
+      <c r="O78" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4155,6 +5253,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L79" t="n">
+        <v>1</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>7Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N79" t="n">
+        <v>3</v>
+      </c>
+      <c r="O79" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4202,6 +5314,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L80" t="n">
+        <v>2</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>7Bring the heat</t>
+        </is>
+      </c>
+      <c r="N80" t="n">
+        <v>4</v>
+      </c>
+      <c r="O80" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4249,6 +5375,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L81" t="n">
+        <v>1</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>7Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N81" t="n">
+        <v>4</v>
+      </c>
+      <c r="O81" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4296,6 +5436,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L82" t="n">
+        <v>2</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>7Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N82" t="n">
+        <v>5</v>
+      </c>
+      <c r="O82" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4343,6 +5497,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L83" t="n">
+        <v>1</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>7Sith Happens</t>
+        </is>
+      </c>
+      <c r="N83" t="n">
+        <v>5</v>
+      </c>
+      <c r="O83" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4390,6 +5558,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L84" t="n">
+        <v>2</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>7Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N84" t="n">
+        <v>6</v>
+      </c>
+      <c r="O84" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4437,6 +5619,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L85" t="n">
+        <v>1</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>7Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N85" t="n">
+        <v>6</v>
+      </c>
+      <c r="O85" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4484,6 +5680,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L86" t="n">
+        <v>2</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>8Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N86" t="n">
+        <v>1</v>
+      </c>
+      <c r="O86" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4531,6 +5741,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L87" t="n">
+        <v>1</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>8Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N87" t="n">
+        <v>1</v>
+      </c>
+      <c r="O87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4578,6 +5802,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L88" t="n">
+        <v>2</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>8Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N88" t="n">
+        <v>2</v>
+      </c>
+      <c r="O88" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4625,6 +5863,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L89" t="n">
+        <v>1</v>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>8Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N89" t="n">
+        <v>2</v>
+      </c>
+      <c r="O89" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4672,6 +5924,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L90" t="n">
+        <v>2</v>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>8Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N90" t="n">
+        <v>3</v>
+      </c>
+      <c r="O90" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4719,6 +5985,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L91" t="n">
+        <v>1</v>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>8Apex Predators</t>
+        </is>
+      </c>
+      <c r="N91" t="n">
+        <v>3</v>
+      </c>
+      <c r="O91" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4766,6 +6046,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L92" t="n">
+        <v>2</v>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>8Sith Happens</t>
+        </is>
+      </c>
+      <c r="N92" t="n">
+        <v>4</v>
+      </c>
+      <c r="O92" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4813,6 +6107,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L93" t="n">
+        <v>1</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>8Bring the heat</t>
+        </is>
+      </c>
+      <c r="N93" t="n">
+        <v>4</v>
+      </c>
+      <c r="O93" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4860,6 +6168,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L94" t="n">
+        <v>2</v>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>8Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N94" t="n">
+        <v>5</v>
+      </c>
+      <c r="O94" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4907,6 +6229,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L95" t="n">
+        <v>1</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>8Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N95" t="n">
+        <v>5</v>
+      </c>
+      <c r="O95" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4954,6 +6290,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L96" t="n">
+        <v>2</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>8Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N96" t="n">
+        <v>6</v>
+      </c>
+      <c r="O96" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5001,6 +6351,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L97" t="n">
+        <v>1</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>8Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N97" t="n">
+        <v>6</v>
+      </c>
+      <c r="O97" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5048,6 +6412,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L98" t="n">
+        <v>2</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>9Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N98" t="n">
+        <v>1</v>
+      </c>
+      <c r="O98" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5095,6 +6473,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L99" t="n">
+        <v>1</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>9Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N99" t="n">
+        <v>1</v>
+      </c>
+      <c r="O99" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5142,6 +6534,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L100" t="n">
+        <v>2</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>9Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N100" t="n">
+        <v>2</v>
+      </c>
+      <c r="O100" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5189,6 +6595,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L101" t="n">
+        <v>1</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>9Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N101" t="n">
+        <v>2</v>
+      </c>
+      <c r="O101" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5236,6 +6656,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L102" t="n">
+        <v>2</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>9Apex Predators</t>
+        </is>
+      </c>
+      <c r="N102" t="n">
+        <v>3</v>
+      </c>
+      <c r="O102" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5283,6 +6717,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L103" t="n">
+        <v>1</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>9Sith Happens</t>
+        </is>
+      </c>
+      <c r="N103" t="n">
+        <v>3</v>
+      </c>
+      <c r="O103" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5330,6 +6778,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L104" t="n">
+        <v>2</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>9Bring the heat</t>
+        </is>
+      </c>
+      <c r="N104" t="n">
+        <v>4</v>
+      </c>
+      <c r="O104" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5377,6 +6839,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L105" t="n">
+        <v>1</v>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>9Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N105" t="n">
+        <v>4</v>
+      </c>
+      <c r="O105" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5424,6 +6900,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L106" t="n">
+        <v>2</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>9Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N106" t="n">
+        <v>5</v>
+      </c>
+      <c r="O106" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5471,6 +6961,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L107" t="n">
+        <v>1</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>9Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N107" t="n">
+        <v>5</v>
+      </c>
+      <c r="O107" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5518,6 +7022,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L108" t="n">
+        <v>2</v>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>9Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N108" t="n">
+        <v>6</v>
+      </c>
+      <c r="O108" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5565,6 +7083,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L109" t="n">
+        <v>1</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>9Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N109" t="n">
+        <v>6</v>
+      </c>
+      <c r="O109" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5612,6 +7144,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L110" t="n">
+        <v>2</v>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>10Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N110" t="n">
+        <v>1</v>
+      </c>
+      <c r="O110" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5659,6 +7205,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L111" t="n">
+        <v>1</v>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>10Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N111" t="n">
+        <v>1</v>
+      </c>
+      <c r="O111" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5706,6 +7266,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L112" t="n">
+        <v>2</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>10Sith Happens</t>
+        </is>
+      </c>
+      <c r="N112" t="n">
+        <v>2</v>
+      </c>
+      <c r="O112" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5753,6 +7327,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L113" t="n">
+        <v>1</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>10Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N113" t="n">
+        <v>2</v>
+      </c>
+      <c r="O113" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5800,6 +7388,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L114" t="n">
+        <v>2</v>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>10Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N114" t="n">
+        <v>3</v>
+      </c>
+      <c r="O114" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5847,6 +7449,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L115" t="n">
+        <v>1</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>10Apex Predators</t>
+        </is>
+      </c>
+      <c r="N115" t="n">
+        <v>3</v>
+      </c>
+      <c r="O115" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5894,6 +7510,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L116" t="n">
+        <v>2</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>10Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N116" t="n">
+        <v>4</v>
+      </c>
+      <c r="O116" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5941,6 +7571,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L117" t="n">
+        <v>1</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>10Bring the heat</t>
+        </is>
+      </c>
+      <c r="N117" t="n">
+        <v>4</v>
+      </c>
+      <c r="O117" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5988,6 +7632,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L118" t="n">
+        <v>2</v>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>10Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N118" t="n">
+        <v>5</v>
+      </c>
+      <c r="O118" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6035,6 +7693,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L119" t="n">
+        <v>1</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>10Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N119" t="n">
+        <v>5</v>
+      </c>
+      <c r="O119" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -6082,6 +7754,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L120" t="n">
+        <v>2</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>10Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N120" t="n">
+        <v>6</v>
+      </c>
+      <c r="O120" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6129,6 +7815,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L121" t="n">
+        <v>1</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>10Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N121" t="n">
+        <v>6</v>
+      </c>
+      <c r="O121" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -6176,6 +7876,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L122" t="n">
+        <v>2</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>11Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N122" t="n">
+        <v>1</v>
+      </c>
+      <c r="O122" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -6223,6 +7937,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L123" t="n">
+        <v>1</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>11Sith Happens</t>
+        </is>
+      </c>
+      <c r="N123" t="n">
+        <v>1</v>
+      </c>
+      <c r="O123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -6270,6 +7998,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L124" t="n">
+        <v>2</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>11Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N124" t="n">
+        <v>2</v>
+      </c>
+      <c r="O124" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -6317,6 +8059,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L125" t="n">
+        <v>1</v>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>11Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N125" t="n">
+        <v>2</v>
+      </c>
+      <c r="O125" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -6364,6 +8120,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L126" t="n">
+        <v>2</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>11Apex Predators</t>
+        </is>
+      </c>
+      <c r="N126" t="n">
+        <v>3</v>
+      </c>
+      <c r="O126" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -6411,6 +8181,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L127" t="n">
+        <v>1</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>11Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N127" t="n">
+        <v>3</v>
+      </c>
+      <c r="O127" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -6458,6 +8242,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L128" t="n">
+        <v>2</v>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>11Bring the heat</t>
+        </is>
+      </c>
+      <c r="N128" t="n">
+        <v>4</v>
+      </c>
+      <c r="O128" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -6505,6 +8303,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L129" t="n">
+        <v>1</v>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>11Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N129" t="n">
+        <v>4</v>
+      </c>
+      <c r="O129" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6552,6 +8364,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L130" t="n">
+        <v>2</v>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>11Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N130" t="n">
+        <v>5</v>
+      </c>
+      <c r="O130" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -6599,6 +8425,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L131" t="n">
+        <v>1</v>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>11Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N131" t="n">
+        <v>5</v>
+      </c>
+      <c r="O131" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -6646,6 +8486,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L132" t="n">
+        <v>2</v>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>11Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N132" t="n">
+        <v>6</v>
+      </c>
+      <c r="O132" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -6693,6 +8547,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L133" t="n">
+        <v>1</v>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>11Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N133" t="n">
+        <v>6</v>
+      </c>
+      <c r="O133" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -6740,6 +8608,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L134" t="n">
+        <v>2</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>12Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N134" t="n">
+        <v>1</v>
+      </c>
+      <c r="O134" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -6787,6 +8669,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L135" t="n">
+        <v>1</v>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>12Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N135" t="n">
+        <v>1</v>
+      </c>
+      <c r="O135" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6834,6 +8730,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L136" t="n">
+        <v>2</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>12Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N136" t="n">
+        <v>2</v>
+      </c>
+      <c r="O136" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -6881,6 +8791,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L137" t="n">
+        <v>1</v>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>12Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N137" t="n">
+        <v>2</v>
+      </c>
+      <c r="O137" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -6928,6 +8852,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L138" t="n">
+        <v>2</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>12Apex Predators</t>
+        </is>
+      </c>
+      <c r="N138" t="n">
+        <v>3</v>
+      </c>
+      <c r="O138" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -6975,6 +8913,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L139" t="n">
+        <v>1</v>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>12Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N139" t="n">
+        <v>3</v>
+      </c>
+      <c r="O139" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -7022,6 +8974,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L140" t="n">
+        <v>2</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>12Bring the heat</t>
+        </is>
+      </c>
+      <c r="N140" t="n">
+        <v>4</v>
+      </c>
+      <c r="O140" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -7069,6 +9035,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L141" t="n">
+        <v>1</v>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>12Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N141" t="n">
+        <v>4</v>
+      </c>
+      <c r="O141" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -7116,6 +9096,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L142" t="n">
+        <v>2</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>12Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N142" t="n">
+        <v>5</v>
+      </c>
+      <c r="O142" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -7163,6 +9157,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L143" t="n">
+        <v>1</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>12Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N143" t="n">
+        <v>5</v>
+      </c>
+      <c r="O143" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -7210,6 +9218,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L144" t="n">
+        <v>2</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>12Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N144" t="n">
+        <v>6</v>
+      </c>
+      <c r="O144" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -7257,6 +9279,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L145" t="n">
+        <v>1</v>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>12Sith Happens</t>
+        </is>
+      </c>
+      <c r="N145" t="n">
+        <v>6</v>
+      </c>
+      <c r="O145" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -7304,6 +9340,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L146" t="n">
+        <v>2</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>13Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>1</v>
+      </c>
+      <c r="O146" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -7351,6 +9401,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L147" t="n">
+        <v>1</v>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>13Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N147" t="n">
+        <v>1</v>
+      </c>
+      <c r="O147" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -7398,6 +9462,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L148" t="n">
+        <v>2</v>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>13Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N148" t="n">
+        <v>2</v>
+      </c>
+      <c r="O148" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -7445,6 +9523,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L149" t="n">
+        <v>1</v>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>13Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N149" t="n">
+        <v>2</v>
+      </c>
+      <c r="O149" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -7492,6 +9584,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L150" t="n">
+        <v>2</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>13Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N150" t="n">
+        <v>3</v>
+      </c>
+      <c r="O150" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -7539,6 +9645,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L151" t="n">
+        <v>1</v>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>13Apex Predators</t>
+        </is>
+      </c>
+      <c r="N151" t="n">
+        <v>3</v>
+      </c>
+      <c r="O151" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -7586,6 +9706,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L152" t="n">
+        <v>2</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>13Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N152" t="n">
+        <v>4</v>
+      </c>
+      <c r="O152" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -7633,6 +9767,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L153" t="n">
+        <v>1</v>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>13Bring the heat</t>
+        </is>
+      </c>
+      <c r="N153" t="n">
+        <v>4</v>
+      </c>
+      <c r="O153" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -7680,6 +9828,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L154" t="n">
+        <v>2</v>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>13Sith Happens</t>
+        </is>
+      </c>
+      <c r="N154" t="n">
+        <v>5</v>
+      </c>
+      <c r="O154" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -7727,6 +9889,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L155" t="n">
+        <v>1</v>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>13Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N155" t="n">
+        <v>5</v>
+      </c>
+      <c r="O155" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -7774,6 +9950,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L156" t="n">
+        <v>2</v>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>13Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N156" t="n">
+        <v>6</v>
+      </c>
+      <c r="O156" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -7821,6 +10011,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L157" t="n">
+        <v>1</v>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>13Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N157" t="n">
+        <v>6</v>
+      </c>
+      <c r="O157" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -7868,6 +10072,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L158" t="n">
+        <v>2</v>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>14Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N158" t="n">
+        <v>1</v>
+      </c>
+      <c r="O158" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -7915,6 +10133,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L159" t="n">
+        <v>1</v>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>14Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N159" t="n">
+        <v>1</v>
+      </c>
+      <c r="O159" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -7962,6 +10194,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L160" t="n">
+        <v>2</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>14Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N160" t="n">
+        <v>2</v>
+      </c>
+      <c r="O160" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -8009,6 +10255,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L161" t="n">
+        <v>1</v>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>14Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N161" t="n">
+        <v>2</v>
+      </c>
+      <c r="O161" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -8056,6 +10316,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L162" t="n">
+        <v>2</v>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>14Apex Predators</t>
+        </is>
+      </c>
+      <c r="N162" t="n">
+        <v>3</v>
+      </c>
+      <c r="O162" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -8103,6 +10377,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L163" t="n">
+        <v>1</v>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>14Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N163" t="n">
+        <v>3</v>
+      </c>
+      <c r="O163" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -8150,6 +10438,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L164" t="n">
+        <v>2</v>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>14Bring the heat</t>
+        </is>
+      </c>
+      <c r="N164" t="n">
+        <v>4</v>
+      </c>
+      <c r="O164" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -8197,6 +10499,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L165" t="n">
+        <v>1</v>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>14Sith Happens</t>
+        </is>
+      </c>
+      <c r="N165" t="n">
+        <v>4</v>
+      </c>
+      <c r="O165" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -8244,6 +10560,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L166" t="n">
+        <v>2</v>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>14Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N166" t="n">
+        <v>5</v>
+      </c>
+      <c r="O166" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -8291,6 +10621,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L167" t="n">
+        <v>1</v>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>14Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N167" t="n">
+        <v>5</v>
+      </c>
+      <c r="O167" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -8338,6 +10682,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L168" t="n">
+        <v>2</v>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>14Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N168" t="n">
+        <v>6</v>
+      </c>
+      <c r="O168" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -8385,6 +10743,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L169" t="n">
+        <v>1</v>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>14Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N169" t="n">
+        <v>6</v>
+      </c>
+      <c r="O169" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -8432,6 +10804,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L170" t="n">
+        <v>2</v>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>15Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N170" t="n">
+        <v>1</v>
+      </c>
+      <c r="O170" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -8479,6 +10865,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L171" t="n">
+        <v>1</v>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>15Bye1</t>
+        </is>
+      </c>
+      <c r="N171" t="n">
+        <v>1</v>
+      </c>
+      <c r="O171" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -8526,6 +10926,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L172" t="n">
+        <v>2</v>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>15Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N172" t="n">
+        <v>2</v>
+      </c>
+      <c r="O172" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -8573,6 +10987,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L173" t="n">
+        <v>1</v>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>15Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N173" t="n">
+        <v>2</v>
+      </c>
+      <c r="O173" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -8620,6 +11048,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L174" t="n">
+        <v>2</v>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>15Sith Happens</t>
+        </is>
+      </c>
+      <c r="N174" t="n">
+        <v>3</v>
+      </c>
+      <c r="O174" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -8667,6 +11109,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L175" t="n">
+        <v>1</v>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>15Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N175" t="n">
+        <v>3</v>
+      </c>
+      <c r="O175" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -8714,6 +11170,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L176" t="n">
+        <v>2</v>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>15Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N176" t="n">
+        <v>4</v>
+      </c>
+      <c r="O176" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -8761,6 +11231,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L177" t="n">
+        <v>1</v>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>15Bye2</t>
+        </is>
+      </c>
+      <c r="N177" t="n">
+        <v>4</v>
+      </c>
+      <c r="O177" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -8808,6 +11292,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L178" t="n">
+        <v>2</v>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>15Apex Predators</t>
+        </is>
+      </c>
+      <c r="N178" t="n">
+        <v>5</v>
+      </c>
+      <c r="O178" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -8855,6 +11353,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L179" t="n">
+        <v>1</v>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>15Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N179" t="n">
+        <v>5</v>
+      </c>
+      <c r="O179" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -8902,6 +11414,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L180" t="n">
+        <v>2</v>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>15Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N180" t="n">
+        <v>6</v>
+      </c>
+      <c r="O180" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -8949,6 +11475,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L181" t="n">
+        <v>1</v>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>15Bring the heat</t>
+        </is>
+      </c>
+      <c r="N181" t="n">
+        <v>6</v>
+      </c>
+      <c r="O181" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -8996,6 +11536,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L182" t="n">
+        <v>2</v>
+      </c>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t>16Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N182" t="n">
+        <v>1</v>
+      </c>
+      <c r="O182" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -9043,6 +11597,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L183" t="n">
+        <v>1</v>
+      </c>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t>16Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N183" t="n">
+        <v>1</v>
+      </c>
+      <c r="O183" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -9090,6 +11658,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L184" t="n">
+        <v>2</v>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>16Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N184" t="n">
+        <v>2</v>
+      </c>
+      <c r="O184" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -9137,6 +11719,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L185" t="n">
+        <v>1</v>
+      </c>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>16Sith Happens</t>
+        </is>
+      </c>
+      <c r="N185" t="n">
+        <v>2</v>
+      </c>
+      <c r="O185" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -9184,6 +11780,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L186" t="n">
+        <v>2</v>
+      </c>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t>16Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N186" t="n">
+        <v>3</v>
+      </c>
+      <c r="O186" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -9231,6 +11841,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L187" t="n">
+        <v>1</v>
+      </c>
+      <c r="M187" t="inlineStr">
+        <is>
+          <t>16Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N187" t="n">
+        <v>3</v>
+      </c>
+      <c r="O187" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -9278,6 +11902,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L188" t="n">
+        <v>2</v>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>16Apex Predators</t>
+        </is>
+      </c>
+      <c r="N188" t="n">
+        <v>4</v>
+      </c>
+      <c r="O188" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -9325,6 +11963,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L189" t="n">
+        <v>1</v>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>16Bring the heat</t>
+        </is>
+      </c>
+      <c r="N189" t="n">
+        <v>4</v>
+      </c>
+      <c r="O189" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -9372,6 +12024,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L190" t="n">
+        <v>2</v>
+      </c>
+      <c r="M190" t="inlineStr">
+        <is>
+          <t>16Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N190" t="n">
+        <v>5</v>
+      </c>
+      <c r="O190" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -9419,6 +12085,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L191" t="n">
+        <v>1</v>
+      </c>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t>16Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N191" t="n">
+        <v>5</v>
+      </c>
+      <c r="O191" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -9466,6 +12146,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L192" t="n">
+        <v>2</v>
+      </c>
+      <c r="M192" t="inlineStr">
+        <is>
+          <t>16Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N192" t="n">
+        <v>6</v>
+      </c>
+      <c r="O192" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -9513,6 +12207,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L193" t="n">
+        <v>1</v>
+      </c>
+      <c r="M193" t="inlineStr">
+        <is>
+          <t>16Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N193" t="n">
+        <v>6</v>
+      </c>
+      <c r="O193" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -9560,6 +12268,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L194" t="n">
+        <v>2</v>
+      </c>
+      <c r="M194" t="inlineStr">
+        <is>
+          <t>17Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N194" t="n">
+        <v>1</v>
+      </c>
+      <c r="O194" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -9607,6 +12329,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L195" t="n">
+        <v>1</v>
+      </c>
+      <c r="M195" t="inlineStr">
+        <is>
+          <t>17Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N195" t="n">
+        <v>1</v>
+      </c>
+      <c r="O195" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -9654,6 +12390,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L196" t="n">
+        <v>2</v>
+      </c>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t>17Sith Happens</t>
+        </is>
+      </c>
+      <c r="N196" t="n">
+        <v>2</v>
+      </c>
+      <c r="O196" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -9701,6 +12451,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L197" t="n">
+        <v>1</v>
+      </c>
+      <c r="M197" t="inlineStr">
+        <is>
+          <t>17Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N197" t="n">
+        <v>2</v>
+      </c>
+      <c r="O197" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -9748,6 +12512,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L198" t="n">
+        <v>2</v>
+      </c>
+      <c r="M198" t="inlineStr">
+        <is>
+          <t>17Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N198" t="n">
+        <v>3</v>
+      </c>
+      <c r="O198" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -9795,6 +12573,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L199" t="n">
+        <v>1</v>
+      </c>
+      <c r="M199" t="inlineStr">
+        <is>
+          <t>17Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N199" t="n">
+        <v>3</v>
+      </c>
+      <c r="O199" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -9842,6 +12634,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L200" t="n">
+        <v>2</v>
+      </c>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t>17Apex Predators</t>
+        </is>
+      </c>
+      <c r="N200" t="n">
+        <v>4</v>
+      </c>
+      <c r="O200" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -9889,6 +12695,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L201" t="n">
+        <v>1</v>
+      </c>
+      <c r="M201" t="inlineStr">
+        <is>
+          <t>17Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N201" t="n">
+        <v>4</v>
+      </c>
+      <c r="O201" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -9936,6 +12756,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L202" t="n">
+        <v>2</v>
+      </c>
+      <c r="M202" t="inlineStr">
+        <is>
+          <t>17Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N202" t="n">
+        <v>5</v>
+      </c>
+      <c r="O202" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -9983,6 +12817,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L203" t="n">
+        <v>1</v>
+      </c>
+      <c r="M203" t="inlineStr">
+        <is>
+          <t>17Bring the heat</t>
+        </is>
+      </c>
+      <c r="N203" t="n">
+        <v>5</v>
+      </c>
+      <c r="O203" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -10030,6 +12878,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L204" t="n">
+        <v>2</v>
+      </c>
+      <c r="M204" t="inlineStr">
+        <is>
+          <t>17Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N204" t="n">
+        <v>6</v>
+      </c>
+      <c r="O204" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -10077,6 +12939,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L205" t="n">
+        <v>1</v>
+      </c>
+      <c r="M205" t="inlineStr">
+        <is>
+          <t>17Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N205" t="n">
+        <v>6</v>
+      </c>
+      <c r="O205" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -10124,6 +13000,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L206" t="n">
+        <v>2</v>
+      </c>
+      <c r="M206" t="inlineStr">
+        <is>
+          <t>18Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="N206" t="n">
+        <v>1</v>
+      </c>
+      <c r="O206" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -10171,6 +13061,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L207" t="n">
+        <v>1</v>
+      </c>
+      <c r="M207" t="inlineStr">
+        <is>
+          <t>18Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="N207" t="n">
+        <v>1</v>
+      </c>
+      <c r="O207" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -10218,6 +13122,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L208" t="n">
+        <v>2</v>
+      </c>
+      <c r="M208" t="inlineStr">
+        <is>
+          <t>18Sith Happens</t>
+        </is>
+      </c>
+      <c r="N208" t="n">
+        <v>2</v>
+      </c>
+      <c r="O208" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -10265,6 +13183,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L209" t="n">
+        <v>1</v>
+      </c>
+      <c r="M209" t="inlineStr">
+        <is>
+          <t>18Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="N209" t="n">
+        <v>2</v>
+      </c>
+      <c r="O209" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -10312,6 +13244,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L210" t="n">
+        <v>2</v>
+      </c>
+      <c r="M210" t="inlineStr">
+        <is>
+          <t>18Drafted by AI</t>
+        </is>
+      </c>
+      <c r="N210" t="n">
+        <v>3</v>
+      </c>
+      <c r="O210" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -10359,6 +13305,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L211" t="n">
+        <v>1</v>
+      </c>
+      <c r="M211" t="inlineStr">
+        <is>
+          <t>18Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="N211" t="n">
+        <v>3</v>
+      </c>
+      <c r="O211" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -10406,6 +13366,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L212" t="n">
+        <v>2</v>
+      </c>
+      <c r="M212" t="inlineStr">
+        <is>
+          <t>18Apex Predators</t>
+        </is>
+      </c>
+      <c r="N212" t="n">
+        <v>4</v>
+      </c>
+      <c r="O212" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -10453,6 +13427,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L213" t="n">
+        <v>1</v>
+      </c>
+      <c r="M213" t="inlineStr">
+        <is>
+          <t>18Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="N213" t="n">
+        <v>4</v>
+      </c>
+      <c r="O213" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -10500,6 +13488,20 @@
           <t>Loss</t>
         </is>
       </c>
+      <c r="L214" t="n">
+        <v>2</v>
+      </c>
+      <c r="M214" t="inlineStr">
+        <is>
+          <t>18Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="N214" t="n">
+        <v>5</v>
+      </c>
+      <c r="O214" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -10547,6 +13549,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L215" t="n">
+        <v>1</v>
+      </c>
+      <c r="M215" t="inlineStr">
+        <is>
+          <t>18Bring the heat</t>
+        </is>
+      </c>
+      <c r="N215" t="n">
+        <v>5</v>
+      </c>
+      <c r="O215" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -10594,6 +13610,20 @@
           <t>Win</t>
         </is>
       </c>
+      <c r="L216" t="n">
+        <v>2</v>
+      </c>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t>18Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N216" t="n">
+        <v>6</v>
+      </c>
+      <c r="O216" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -10640,6 +13670,20 @@
         <is>
           <t>Loss</t>
         </is>
+      </c>
+      <c r="L217" t="n">
+        <v>1</v>
+      </c>
+      <c r="M217" t="inlineStr">
+        <is>
+          <t>18Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="N217" t="n">
+        <v>6</v>
+      </c>
+      <c r="O217" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added final matchup in wk 15 when there are byes, checked all scores are correct, formatted scoreboard page a bit
</commit_message>
<xml_diff>
--- a/matchups.xlsx
+++ b/matchups.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O217"/>
+  <dimension ref="A1:O219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11493,16 +11493,16 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Mighty Rubber Ducks</t>
+          <t>Kuppenheimer</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -11510,25 +11510,25 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>127.69</v>
+        <v>92.08000000000001</v>
       </c>
       <c r="F182" t="n">
-        <v>150.82</v>
+        <v>132.44</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>WINNERS_BRACKET</t>
+          <t>LOSERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H182" t="n">
-        <v>-2.79</v>
+        <v>-1.99</v>
       </c>
       <c r="I182" t="n">
-        <v>27.18</v>
+        <v>63.28</v>
       </c>
       <c r="J182" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs vs. Mighty Rubber Ducks</t>
+          <t>Boomer Sooners vs. Kuppenheimer</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
@@ -11541,29 +11541,29 @@
       </c>
       <c r="M182" t="inlineStr">
         <is>
-          <t>16Baby Back Gibbs</t>
+          <t>15Boomer Sooners</t>
         </is>
       </c>
       <c r="N182" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O182" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Mighty Rubber Ducks</t>
+          <t>Kuppenheimer</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
@@ -11571,25 +11571,25 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>130.48</v>
+        <v>94.07000000000001</v>
       </c>
       <c r="F183" t="n">
-        <v>123.64</v>
+        <v>69.16</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>WINNERS_BRACKET</t>
+          <t>LOSERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H183" t="n">
-        <v>2.79</v>
+        <v>1.99</v>
       </c>
       <c r="I183" t="n">
-        <v>-27.18</v>
+        <v>-63.28</v>
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs vs. Mighty Rubber Ducks</t>
+          <t>Boomer Sooners vs. Kuppenheimer</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -11602,25 +11602,25 @@
       </c>
       <c r="M183" t="inlineStr">
         <is>
-          <t>16Mighty Rubber Ducks</t>
+          <t>15Kuppenheimer</t>
         </is>
       </c>
       <c r="N183" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O183" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Magic Mikaela</t>
+          <t>Baby Back Gibbs</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Sith Happens</t>
+          <t>Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -11632,10 +11632,10 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>123.32</v>
+        <v>127.69</v>
       </c>
       <c r="F184" t="n">
-        <v>163.34</v>
+        <v>150.82</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -11643,14 +11643,14 @@
         </is>
       </c>
       <c r="H184" t="n">
-        <v>-8</v>
+        <v>-2.79</v>
       </c>
       <c r="I184" t="n">
-        <v>35.5</v>
+        <v>27.18</v>
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>Magic Mikaela vs. Sith Happens</t>
+          <t>Baby Back Gibbs vs. Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -11663,25 +11663,25 @@
       </c>
       <c r="M184" t="inlineStr">
         <is>
-          <t>16Magic Mikaela</t>
+          <t>16Baby Back Gibbs</t>
         </is>
       </c>
       <c r="N184" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O184" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Sith Happens</t>
+          <t>Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Magic Mikaela</t>
+          <t>Baby Back Gibbs</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -11693,10 +11693,10 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>131.32</v>
+        <v>130.48</v>
       </c>
       <c r="F185" t="n">
-        <v>127.84</v>
+        <v>123.64</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -11704,14 +11704,14 @@
         </is>
       </c>
       <c r="H185" t="n">
-        <v>8</v>
+        <v>2.79</v>
       </c>
       <c r="I185" t="n">
-        <v>-35.5</v>
+        <v>-27.18</v>
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>Magic Mikaela vs. Sith Happens</t>
+          <t>Baby Back Gibbs vs. Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -11724,25 +11724,25 @@
       </c>
       <c r="M185" t="inlineStr">
         <is>
-          <t>16Sith Happens</t>
+          <t>16Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="N185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Drafted by AI</t>
+          <t>Magic Mikaela</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Compile and Conquer</t>
+          <t>Sith Happens</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -11754,30 +11754,30 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>109.56</v>
+        <v>123.32</v>
       </c>
       <c r="F186" t="n">
-        <v>108.12</v>
+        <v>163.34</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>WINNERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_BRACKET</t>
         </is>
       </c>
       <c r="H186" t="n">
-        <v>-10.94</v>
+        <v>-8</v>
       </c>
       <c r="I186" t="n">
-        <v>-31.76</v>
+        <v>35.5</v>
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>Drafted by AI vs. Compile and Conquer</t>
+          <t>Magic Mikaela vs. Sith Happens</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L186" t="n">
@@ -11785,25 +11785,25 @@
       </c>
       <c r="M186" t="inlineStr">
         <is>
-          <t>16Drafted by AI</t>
+          <t>16Magic Mikaela</t>
         </is>
       </c>
       <c r="N186" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O186" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Compile and Conquer</t>
+          <t>Sith Happens</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Drafted by AI</t>
+          <t>Magic Mikaela</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -11815,30 +11815,30 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>120.5</v>
+        <v>131.32</v>
       </c>
       <c r="F187" t="n">
-        <v>139.88</v>
+        <v>127.84</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>WINNERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_BRACKET</t>
         </is>
       </c>
       <c r="H187" t="n">
-        <v>10.94</v>
+        <v>8</v>
       </c>
       <c r="I187" t="n">
-        <v>31.76</v>
+        <v>-35.5</v>
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>Drafted by AI vs. Compile and Conquer</t>
+          <t>Magic Mikaela vs. Sith Happens</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L187" t="n">
@@ -11846,25 +11846,25 @@
       </c>
       <c r="M187" t="inlineStr">
         <is>
-          <t>16Compile and Conquer</t>
+          <t>16Sith Happens</t>
         </is>
       </c>
       <c r="N187" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O187" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Apex Predators</t>
+          <t>Drafted by AI</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Bring the heat</t>
+          <t>Compile and Conquer</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -11876,30 +11876,30 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>136.1</v>
+        <v>109.56</v>
       </c>
       <c r="F188" t="n">
-        <v>167.82</v>
+        <v>108.12</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>LOSERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H188" t="n">
-        <v>30.03</v>
+        <v>-10.94</v>
       </c>
       <c r="I188" t="n">
-        <v>68.16</v>
+        <v>-31.76</v>
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>Apex Predators vs. Bring the heat</t>
+          <t>Drafted by AI vs. Compile and Conquer</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L188" t="n">
@@ -11907,25 +11907,25 @@
       </c>
       <c r="M188" t="inlineStr">
         <is>
-          <t>16Apex Predators</t>
+          <t>16Drafted by AI</t>
         </is>
       </c>
       <c r="N188" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O188" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Bring the heat</t>
+          <t>Compile and Conquer</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Apex Predators</t>
+          <t>Drafted by AI</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -11937,30 +11937,30 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>106.07</v>
+        <v>120.5</v>
       </c>
       <c r="F189" t="n">
-        <v>99.66</v>
+        <v>139.88</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>LOSERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H189" t="n">
-        <v>-30.03</v>
+        <v>10.94</v>
       </c>
       <c r="I189" t="n">
-        <v>-68.16</v>
+        <v>31.76</v>
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>Apex Predators vs. Bring the heat</t>
+          <t>Drafted by AI vs. Compile and Conquer</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L189" t="n">
@@ -11968,25 +11968,25 @@
       </c>
       <c r="M189" t="inlineStr">
         <is>
-          <t>16Bring the heat</t>
+          <t>16Compile and Conquer</t>
         </is>
       </c>
       <c r="N189" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O189" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team</t>
+          <t>Apex Predators</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Boomer Sooners</t>
+          <t>Bring the heat</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -11998,10 +11998,10 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>123.41</v>
+        <v>136.1</v>
       </c>
       <c r="F190" t="n">
-        <v>94.3</v>
+        <v>167.82</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -12009,19 +12009,19 @@
         </is>
       </c>
       <c r="H190" t="n">
-        <v>25.82</v>
+        <v>30.03</v>
       </c>
       <c r="I190" t="n">
-        <v>-34.66</v>
+        <v>68.16</v>
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team vs. Boomer Sooners</t>
+          <t>Apex Predators vs. Bring the heat</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L190" t="n">
@@ -12029,25 +12029,25 @@
       </c>
       <c r="M190" t="inlineStr">
         <is>
-          <t>16Aida's Astounding Team</t>
+          <t>16Apex Predators</t>
         </is>
       </c>
       <c r="N190" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O190" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Boomer Sooners</t>
+          <t>Bring the heat</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team</t>
+          <t>Apex Predators</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -12059,10 +12059,10 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>97.59000000000002</v>
+        <v>106.07</v>
       </c>
       <c r="F191" t="n">
-        <v>128.96</v>
+        <v>99.66</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -12070,19 +12070,19 @@
         </is>
       </c>
       <c r="H191" t="n">
-        <v>-25.82</v>
+        <v>-30.03</v>
       </c>
       <c r="I191" t="n">
-        <v>34.66</v>
+        <v>-68.16</v>
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team vs. Boomer Sooners</t>
+          <t>Apex Predators vs. Bring the heat</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L191" t="n">
@@ -12090,25 +12090,25 @@
       </c>
       <c r="M191" t="inlineStr">
         <is>
-          <t>16Boomer Sooners</t>
+          <t>16Bring the heat</t>
         </is>
       </c>
       <c r="N191" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O191" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team</t>
+          <t>Aida's Astounding Team</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Kuppenheimer</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -12120,10 +12120,10 @@
         </is>
       </c>
       <c r="E192" t="n">
-        <v>113.17</v>
+        <v>123.41</v>
       </c>
       <c r="F192" t="n">
-        <v>125.06</v>
+        <v>94.3</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -12131,19 +12131,19 @@
         </is>
       </c>
       <c r="H192" t="n">
-        <v>12.11</v>
+        <v>25.82</v>
       </c>
       <c r="I192" t="n">
-        <v>32.28</v>
+        <v>-34.66</v>
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team vs. Kuppenheimer</t>
+          <t>Aida's Astounding Team vs. Boomer Sooners</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L192" t="n">
@@ -12151,25 +12151,25 @@
       </c>
       <c r="M192" t="inlineStr">
         <is>
-          <t>16Kelly's Deluxe Team</t>
+          <t>16Aida's Astounding Team</t>
         </is>
       </c>
       <c r="N192" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O192" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Kuppenheimer</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team</t>
+          <t>Aida's Astounding Team</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -12181,10 +12181,10 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>101.06</v>
+        <v>97.59000000000002</v>
       </c>
       <c r="F193" t="n">
-        <v>92.78</v>
+        <v>128.96</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -12192,19 +12192,19 @@
         </is>
       </c>
       <c r="H193" t="n">
-        <v>-12.11</v>
+        <v>-25.82</v>
       </c>
       <c r="I193" t="n">
-        <v>-32.28</v>
+        <v>34.66</v>
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team vs. Kuppenheimer</t>
+          <t>Aida's Astounding Team vs. Boomer Sooners</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L193" t="n">
@@ -12212,29 +12212,29 @@
       </c>
       <c r="M193" t="inlineStr">
         <is>
-          <t>16Kuppenheimer</t>
+          <t>16Boomer Sooners</t>
         </is>
       </c>
       <c r="N193" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O193" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs</t>
+          <t>Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Magic Mikaela</t>
+          <t>Kuppenheimer</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
@@ -12242,25 +12242,25 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>159.36</v>
+        <v>113.17</v>
       </c>
       <c r="F194" t="n">
-        <v>159.36</v>
+        <v>125.06</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>WINNERS_BRACKET</t>
+          <t>LOSERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H194" t="n">
-        <v>29.04</v>
+        <v>12.11</v>
       </c>
       <c r="I194" t="n">
-        <v>29.04</v>
+        <v>32.28</v>
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs vs. Magic Mikaela</t>
+          <t>Kelly's Deluxe Team vs. Kuppenheimer</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -12273,29 +12273,29 @@
       </c>
       <c r="M194" t="inlineStr">
         <is>
-          <t>17Baby Back Gibbs</t>
+          <t>16Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="N194" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O194" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Magic Mikaela</t>
+          <t>Kuppenheimer</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs</t>
+          <t>Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D195" t="inlineStr">
         <is>
@@ -12303,25 +12303,25 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>130.32</v>
+        <v>101.06</v>
       </c>
       <c r="F195" t="n">
-        <v>130.32</v>
+        <v>92.78</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>WINNERS_BRACKET</t>
+          <t>LOSERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H195" t="n">
-        <v>-29.04</v>
+        <v>-12.11</v>
       </c>
       <c r="I195" t="n">
-        <v>-29.04</v>
+        <v>-32.28</v>
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs vs. Magic Mikaela</t>
+          <t>Kelly's Deluxe Team vs. Kuppenheimer</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -12334,25 +12334,25 @@
       </c>
       <c r="M195" t="inlineStr">
         <is>
-          <t>17Magic Mikaela</t>
+          <t>16Kuppenheimer</t>
         </is>
       </c>
       <c r="N195" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O195" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Sith Happens</t>
+          <t>Baby Back Gibbs</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Mighty Rubber Ducks</t>
+          <t>Magic Mikaela</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -12364,25 +12364,25 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>140.88</v>
+        <v>159.36</v>
       </c>
       <c r="F196" t="n">
-        <v>140.88</v>
+        <v>159.36</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>WINNERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_BRACKET</t>
         </is>
       </c>
       <c r="H196" t="n">
-        <v>67.18000000000001</v>
+        <v>29.04</v>
       </c>
       <c r="I196" t="n">
-        <v>67.18000000000001</v>
+        <v>29.04</v>
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>Sith Happens vs. Mighty Rubber Ducks</t>
+          <t>Baby Back Gibbs vs. Magic Mikaela</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -12395,25 +12395,25 @@
       </c>
       <c r="M196" t="inlineStr">
         <is>
-          <t>17Sith Happens</t>
+          <t>17Baby Back Gibbs</t>
         </is>
       </c>
       <c r="N196" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O196" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Mighty Rubber Ducks</t>
+          <t>Magic Mikaela</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Sith Happens</t>
+          <t>Baby Back Gibbs</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -12425,25 +12425,25 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>73.7</v>
+        <v>130.32</v>
       </c>
       <c r="F197" t="n">
-        <v>73.7</v>
+        <v>130.32</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>WINNERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_BRACKET</t>
         </is>
       </c>
       <c r="H197" t="n">
-        <v>-67.18000000000001</v>
+        <v>-29.04</v>
       </c>
       <c r="I197" t="n">
-        <v>-67.18000000000001</v>
+        <v>-29.04</v>
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>Sith Happens vs. Mighty Rubber Ducks</t>
+          <t>Baby Back Gibbs vs. Magic Mikaela</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -12456,25 +12456,25 @@
       </c>
       <c r="M197" t="inlineStr">
         <is>
-          <t>17Mighty Rubber Ducks</t>
+          <t>17Magic Mikaela</t>
         </is>
       </c>
       <c r="N197" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O197" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Drafted by AI</t>
+          <t>Sith Happens</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Compile and Conquer</t>
+          <t>Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -12486,10 +12486,10 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>134.48</v>
+        <v>140.88</v>
       </c>
       <c r="F198" t="n">
-        <v>134.48</v>
+        <v>140.88</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
@@ -12497,19 +12497,19 @@
         </is>
       </c>
       <c r="H198" t="n">
-        <v>-20.8</v>
+        <v>67.18000000000001</v>
       </c>
       <c r="I198" t="n">
-        <v>-20.8</v>
+        <v>67.18000000000001</v>
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>Drafted by AI vs. Compile and Conquer</t>
+          <t>Sith Happens vs. Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L198" t="n">
@@ -12517,25 +12517,25 @@
       </c>
       <c r="M198" t="inlineStr">
         <is>
-          <t>17Drafted by AI</t>
+          <t>17Sith Happens</t>
         </is>
       </c>
       <c r="N198" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O198" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Compile and Conquer</t>
+          <t>Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Drafted by AI</t>
+          <t>Sith Happens</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -12547,10 +12547,10 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>155.28</v>
+        <v>73.7</v>
       </c>
       <c r="F199" t="n">
-        <v>155.28</v>
+        <v>73.7</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
@@ -12558,19 +12558,19 @@
         </is>
       </c>
       <c r="H199" t="n">
-        <v>20.8</v>
+        <v>-67.18000000000001</v>
       </c>
       <c r="I199" t="n">
-        <v>20.8</v>
+        <v>-67.18000000000001</v>
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>Drafted by AI vs. Compile and Conquer</t>
+          <t>Sith Happens vs. Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L199" t="n">
@@ -12578,25 +12578,25 @@
       </c>
       <c r="M199" t="inlineStr">
         <is>
-          <t>17Compile and Conquer</t>
+          <t>17Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="N199" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O199" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Apex Predators</t>
+          <t>Drafted by AI</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Boomer Sooners</t>
+          <t>Compile and Conquer</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -12608,30 +12608,30 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>158.88</v>
+        <v>134.48</v>
       </c>
       <c r="F200" t="n">
-        <v>158.88</v>
+        <v>134.48</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>LOSERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H200" t="n">
-        <v>72.40000000000001</v>
+        <v>-20.8</v>
       </c>
       <c r="I200" t="n">
-        <v>72.40000000000001</v>
+        <v>-20.8</v>
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>Apex Predators vs. Boomer Sooners</t>
+          <t>Drafted by AI vs. Compile and Conquer</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L200" t="n">
@@ -12639,25 +12639,25 @@
       </c>
       <c r="M200" t="inlineStr">
         <is>
-          <t>17Apex Predators</t>
+          <t>17Drafted by AI</t>
         </is>
       </c>
       <c r="N200" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O200" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Boomer Sooners</t>
+          <t>Compile and Conquer</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Apex Predators</t>
+          <t>Drafted by AI</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -12669,30 +12669,30 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>86.48</v>
+        <v>155.28</v>
       </c>
       <c r="F201" t="n">
-        <v>86.48</v>
+        <v>155.28</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>LOSERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H201" t="n">
-        <v>-72.40000000000001</v>
+        <v>20.8</v>
       </c>
       <c r="I201" t="n">
-        <v>-72.40000000000001</v>
+        <v>20.8</v>
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>Apex Predators vs. Boomer Sooners</t>
+          <t>Drafted by AI vs. Compile and Conquer</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L201" t="n">
@@ -12700,25 +12700,25 @@
       </c>
       <c r="M201" t="inlineStr">
         <is>
-          <t>17Boomer Sooners</t>
+          <t>17Compile and Conquer</t>
         </is>
       </c>
       <c r="N201" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O201" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team</t>
+          <t>Apex Predators</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Bring the heat</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -12730,10 +12730,10 @@
         </is>
       </c>
       <c r="E202" t="n">
-        <v>75.7</v>
+        <v>158.88</v>
       </c>
       <c r="F202" t="n">
-        <v>75.7</v>
+        <v>158.88</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
@@ -12741,19 +12741,19 @@
         </is>
       </c>
       <c r="H202" t="n">
-        <v>-33.18</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="I202" t="n">
-        <v>-33.18</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team vs. Bring the heat</t>
+          <t>Apex Predators vs. Boomer Sooners</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L202" t="n">
@@ -12761,25 +12761,25 @@
       </c>
       <c r="M202" t="inlineStr">
         <is>
-          <t>17Kelly's Deluxe Team</t>
+          <t>17Apex Predators</t>
         </is>
       </c>
       <c r="N202" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O202" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Bring the heat</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team</t>
+          <t>Apex Predators</t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -12791,10 +12791,10 @@
         </is>
       </c>
       <c r="E203" t="n">
-        <v>108.88</v>
+        <v>86.48</v>
       </c>
       <c r="F203" t="n">
-        <v>108.88</v>
+        <v>86.48</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -12802,19 +12802,19 @@
         </is>
       </c>
       <c r="H203" t="n">
-        <v>33.18</v>
+        <v>-72.40000000000001</v>
       </c>
       <c r="I203" t="n">
-        <v>33.18</v>
+        <v>-72.40000000000001</v>
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team vs. Bring the heat</t>
+          <t>Apex Predators vs. Boomer Sooners</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L203" t="n">
@@ -12822,25 +12822,25 @@
       </c>
       <c r="M203" t="inlineStr">
         <is>
-          <t>17Bring the heat</t>
+          <t>17Boomer Sooners</t>
         </is>
       </c>
       <c r="N203" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O203" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team</t>
+          <t>Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Kuppenheimer</t>
+          <t>Bring the heat</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -12852,10 +12852,10 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>105.06</v>
+        <v>75.7</v>
       </c>
       <c r="F204" t="n">
-        <v>105.06</v>
+        <v>75.7</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -12863,19 +12863,19 @@
         </is>
       </c>
       <c r="H204" t="n">
-        <v>58.12</v>
+        <v>-33.18</v>
       </c>
       <c r="I204" t="n">
-        <v>58.12</v>
+        <v>-33.18</v>
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team vs. Kuppenheimer</t>
+          <t>Kelly's Deluxe Team vs. Bring the heat</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L204" t="n">
@@ -12883,25 +12883,25 @@
       </c>
       <c r="M204" t="inlineStr">
         <is>
-          <t>17Aida's Astounding Team</t>
+          <t>17Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="N204" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O204" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Kuppenheimer</t>
+          <t>Bring the heat</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team</t>
+          <t>Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -12913,10 +12913,10 @@
         </is>
       </c>
       <c r="E205" t="n">
-        <v>46.94</v>
+        <v>108.88</v>
       </c>
       <c r="F205" t="n">
-        <v>46.94</v>
+        <v>108.88</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
@@ -12924,19 +12924,19 @@
         </is>
       </c>
       <c r="H205" t="n">
-        <v>-58.12</v>
+        <v>33.18</v>
       </c>
       <c r="I205" t="n">
-        <v>-58.12</v>
+        <v>33.18</v>
       </c>
       <c r="J205" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team vs. Kuppenheimer</t>
+          <t>Kelly's Deluxe Team vs. Bring the heat</t>
         </is>
       </c>
       <c r="K205" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L205" t="n">
@@ -12944,29 +12944,29 @@
       </c>
       <c r="M205" t="inlineStr">
         <is>
-          <t>17Kuppenheimer</t>
+          <t>17Bring the heat</t>
         </is>
       </c>
       <c r="N205" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O205" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs</t>
+          <t>Aida's Astounding Team</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Magic Mikaela</t>
+          <t>Kuppenheimer</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -12974,25 +12974,25 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>159.36</v>
+        <v>105.06</v>
       </c>
       <c r="F206" t="n">
-        <v>159.36</v>
+        <v>105.06</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>WINNERS_BRACKET</t>
+          <t>LOSERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H206" t="n">
-        <v>29.04</v>
+        <v>58.12</v>
       </c>
       <c r="I206" t="n">
-        <v>29.04</v>
+        <v>58.12</v>
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs vs. Magic Mikaela</t>
+          <t>Aida's Astounding Team vs. Kuppenheimer</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
@@ -13005,29 +13005,29 @@
       </c>
       <c r="M206" t="inlineStr">
         <is>
-          <t>18Baby Back Gibbs</t>
+          <t>17Aida's Astounding Team</t>
         </is>
       </c>
       <c r="N206" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O206" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Magic Mikaela</t>
+          <t>Kuppenheimer</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs</t>
+          <t>Aida's Astounding Team</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D207" t="inlineStr">
         <is>
@@ -13035,25 +13035,25 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>130.32</v>
+        <v>46.94</v>
       </c>
       <c r="F207" t="n">
-        <v>130.32</v>
+        <v>46.94</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>WINNERS_BRACKET</t>
+          <t>LOSERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H207" t="n">
-        <v>-29.04</v>
+        <v>-58.12</v>
       </c>
       <c r="I207" t="n">
-        <v>-29.04</v>
+        <v>-58.12</v>
       </c>
       <c r="J207" t="inlineStr">
         <is>
-          <t>Baby Back Gibbs vs. Magic Mikaela</t>
+          <t>Aida's Astounding Team vs. Kuppenheimer</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -13066,25 +13066,25 @@
       </c>
       <c r="M207" t="inlineStr">
         <is>
-          <t>18Magic Mikaela</t>
+          <t>17Kuppenheimer</t>
         </is>
       </c>
       <c r="N207" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O207" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Sith Happens</t>
+          <t>Baby Back Gibbs</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Mighty Rubber Ducks</t>
+          <t>Magic Mikaela</t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -13096,25 +13096,25 @@
         </is>
       </c>
       <c r="E208" t="n">
-        <v>140.88</v>
+        <v>159.36</v>
       </c>
       <c r="F208" t="n">
-        <v>140.88</v>
+        <v>159.36</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>WINNERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_BRACKET</t>
         </is>
       </c>
       <c r="H208" t="n">
-        <v>67.18000000000001</v>
+        <v>29.04</v>
       </c>
       <c r="I208" t="n">
-        <v>67.18000000000001</v>
+        <v>29.04</v>
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>Sith Happens vs. Mighty Rubber Ducks</t>
+          <t>Baby Back Gibbs vs. Magic Mikaela</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -13127,25 +13127,25 @@
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>18Sith Happens</t>
+          <t>18Baby Back Gibbs</t>
         </is>
       </c>
       <c r="N208" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O208" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Mighty Rubber Ducks</t>
+          <t>Magic Mikaela</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Sith Happens</t>
+          <t>Baby Back Gibbs</t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -13157,25 +13157,25 @@
         </is>
       </c>
       <c r="E209" t="n">
-        <v>73.7</v>
+        <v>130.32</v>
       </c>
       <c r="F209" t="n">
-        <v>73.7</v>
+        <v>130.32</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>WINNERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_BRACKET</t>
         </is>
       </c>
       <c r="H209" t="n">
-        <v>-67.18000000000001</v>
+        <v>-29.04</v>
       </c>
       <c r="I209" t="n">
-        <v>-67.18000000000001</v>
+        <v>-29.04</v>
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>Sith Happens vs. Mighty Rubber Ducks</t>
+          <t>Baby Back Gibbs vs. Magic Mikaela</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -13188,25 +13188,25 @@
       </c>
       <c r="M209" t="inlineStr">
         <is>
-          <t>18Mighty Rubber Ducks</t>
+          <t>18Magic Mikaela</t>
         </is>
       </c>
       <c r="N209" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O209" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Drafted by AI</t>
+          <t>Sith Happens</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Compile and Conquer</t>
+          <t>Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -13218,10 +13218,10 @@
         </is>
       </c>
       <c r="E210" t="n">
-        <v>134.48</v>
+        <v>140.88</v>
       </c>
       <c r="F210" t="n">
-        <v>134.48</v>
+        <v>140.88</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -13229,19 +13229,19 @@
         </is>
       </c>
       <c r="H210" t="n">
-        <v>-20.8</v>
+        <v>67.18000000000001</v>
       </c>
       <c r="I210" t="n">
-        <v>-20.8</v>
+        <v>67.18000000000001</v>
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>Drafted by AI vs. Compile and Conquer</t>
+          <t>Sith Happens vs. Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L210" t="n">
@@ -13249,25 +13249,25 @@
       </c>
       <c r="M210" t="inlineStr">
         <is>
-          <t>18Drafted by AI</t>
+          <t>18Sith Happens</t>
         </is>
       </c>
       <c r="N210" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O210" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Compile and Conquer</t>
+          <t>Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Drafted by AI</t>
+          <t>Sith Happens</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -13279,10 +13279,10 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>155.28</v>
+        <v>73.7</v>
       </c>
       <c r="F211" t="n">
-        <v>155.28</v>
+        <v>73.7</v>
       </c>
       <c r="G211" t="inlineStr">
         <is>
@@ -13290,19 +13290,19 @@
         </is>
       </c>
       <c r="H211" t="n">
-        <v>20.8</v>
+        <v>-67.18000000000001</v>
       </c>
       <c r="I211" t="n">
-        <v>20.8</v>
+        <v>-67.18000000000001</v>
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>Drafted by AI vs. Compile and Conquer</t>
+          <t>Sith Happens vs. Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L211" t="n">
@@ -13310,25 +13310,25 @@
       </c>
       <c r="M211" t="inlineStr">
         <is>
-          <t>18Compile and Conquer</t>
+          <t>18Mighty Rubber Ducks</t>
         </is>
       </c>
       <c r="N211" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O211" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Apex Predators</t>
+          <t>Drafted by AI</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Boomer Sooners</t>
+          <t>Compile and Conquer</t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -13340,30 +13340,30 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>158.88</v>
+        <v>134.48</v>
       </c>
       <c r="F212" t="n">
-        <v>158.88</v>
+        <v>134.48</v>
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>LOSERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H212" t="n">
-        <v>72.40000000000001</v>
+        <v>-20.8</v>
       </c>
       <c r="I212" t="n">
-        <v>72.40000000000001</v>
+        <v>-20.8</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
-          <t>Apex Predators vs. Boomer Sooners</t>
+          <t>Drafted by AI vs. Compile and Conquer</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L212" t="n">
@@ -13371,25 +13371,25 @@
       </c>
       <c r="M212" t="inlineStr">
         <is>
-          <t>18Apex Predators</t>
+          <t>18Drafted by AI</t>
         </is>
       </c>
       <c r="N212" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O212" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Boomer Sooners</t>
+          <t>Compile and Conquer</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Apex Predators</t>
+          <t>Drafted by AI</t>
         </is>
       </c>
       <c r="C213" t="n">
@@ -13401,30 +13401,30 @@
         </is>
       </c>
       <c r="E213" t="n">
-        <v>86.48</v>
+        <v>155.28</v>
       </c>
       <c r="F213" t="n">
-        <v>86.48</v>
+        <v>155.28</v>
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>LOSERS_CONSOLATION_LADDER</t>
+          <t>WINNERS_CONSOLATION_LADDER</t>
         </is>
       </c>
       <c r="H213" t="n">
-        <v>-72.40000000000001</v>
+        <v>20.8</v>
       </c>
       <c r="I213" t="n">
-        <v>-72.40000000000001</v>
+        <v>20.8</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>Apex Predators vs. Boomer Sooners</t>
+          <t>Drafted by AI vs. Compile and Conquer</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L213" t="n">
@@ -13432,25 +13432,25 @@
       </c>
       <c r="M213" t="inlineStr">
         <is>
-          <t>18Boomer Sooners</t>
+          <t>18Compile and Conquer</t>
         </is>
       </c>
       <c r="N213" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O213" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team</t>
+          <t>Apex Predators</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Bring the heat</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="C214" t="n">
@@ -13462,10 +13462,10 @@
         </is>
       </c>
       <c r="E214" t="n">
-        <v>75.7</v>
+        <v>158.88</v>
       </c>
       <c r="F214" t="n">
-        <v>75.7</v>
+        <v>158.88</v>
       </c>
       <c r="G214" t="inlineStr">
         <is>
@@ -13473,19 +13473,19 @@
         </is>
       </c>
       <c r="H214" t="n">
-        <v>-33.18</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="I214" t="n">
-        <v>-33.18</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team vs. Bring the heat</t>
+          <t>Apex Predators vs. Boomer Sooners</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Win</t>
         </is>
       </c>
       <c r="L214" t="n">
@@ -13493,25 +13493,25 @@
       </c>
       <c r="M214" t="inlineStr">
         <is>
-          <t>18Kelly's Deluxe Team</t>
+          <t>18Apex Predators</t>
         </is>
       </c>
       <c r="N214" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O214" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Bring the heat</t>
+          <t>Boomer Sooners</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team</t>
+          <t>Apex Predators</t>
         </is>
       </c>
       <c r="C215" t="n">
@@ -13523,10 +13523,10 @@
         </is>
       </c>
       <c r="E215" t="n">
-        <v>108.88</v>
+        <v>86.48</v>
       </c>
       <c r="F215" t="n">
-        <v>108.88</v>
+        <v>86.48</v>
       </c>
       <c r="G215" t="inlineStr">
         <is>
@@ -13534,19 +13534,19 @@
         </is>
       </c>
       <c r="H215" t="n">
-        <v>33.18</v>
+        <v>-72.40000000000001</v>
       </c>
       <c r="I215" t="n">
-        <v>33.18</v>
+        <v>-72.40000000000001</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>Kelly's Deluxe Team vs. Bring the heat</t>
+          <t>Apex Predators vs. Boomer Sooners</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L215" t="n">
@@ -13554,25 +13554,25 @@
       </c>
       <c r="M215" t="inlineStr">
         <is>
-          <t>18Bring the heat</t>
+          <t>18Boomer Sooners</t>
         </is>
       </c>
       <c r="N215" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O215" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team</t>
+          <t>Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Kuppenheimer</t>
+          <t>Bring the heat</t>
         </is>
       </c>
       <c r="C216" t="n">
@@ -13584,10 +13584,10 @@
         </is>
       </c>
       <c r="E216" t="n">
-        <v>105.06</v>
+        <v>75.7</v>
       </c>
       <c r="F216" t="n">
-        <v>105.06</v>
+        <v>75.7</v>
       </c>
       <c r="G216" t="inlineStr">
         <is>
@@ -13595,19 +13595,19 @@
         </is>
       </c>
       <c r="H216" t="n">
-        <v>58.12</v>
+        <v>-33.18</v>
       </c>
       <c r="I216" t="n">
-        <v>58.12</v>
+        <v>-33.18</v>
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team vs. Kuppenheimer</t>
+          <t>Kelly's Deluxe Team vs. Bring the heat</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
         <is>
-          <t>Win</t>
+          <t>Loss</t>
         </is>
       </c>
       <c r="L216" t="n">
@@ -13615,25 +13615,25 @@
       </c>
       <c r="M216" t="inlineStr">
         <is>
-          <t>18Aida's Astounding Team</t>
+          <t>18Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="N216" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O216" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Kuppenheimer</t>
+          <t>Bring the heat</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Aida's Astounding Team</t>
+          <t>Kelly's Deluxe Team</t>
         </is>
       </c>
       <c r="C217" t="n">
@@ -13645,44 +13645,166 @@
         </is>
       </c>
       <c r="E217" t="n">
+        <v>108.88</v>
+      </c>
+      <c r="F217" t="n">
+        <v>108.88</v>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>LOSERS_CONSOLATION_LADDER</t>
+        </is>
+      </c>
+      <c r="H217" t="n">
+        <v>33.18</v>
+      </c>
+      <c r="I217" t="n">
+        <v>33.18</v>
+      </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>Kelly's Deluxe Team vs. Bring the heat</t>
+        </is>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="L217" t="n">
+        <v>1</v>
+      </c>
+      <c r="M217" t="inlineStr">
+        <is>
+          <t>18Bring the heat</t>
+        </is>
+      </c>
+      <c r="N217" t="n">
+        <v>5</v>
+      </c>
+      <c r="O217" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
+        <v>18</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>105.06</v>
+      </c>
+      <c r="F218" t="n">
+        <v>105.06</v>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>LOSERS_CONSOLATION_LADDER</t>
+        </is>
+      </c>
+      <c r="H218" t="n">
+        <v>58.12</v>
+      </c>
+      <c r="I218" t="n">
+        <v>58.12</v>
+      </c>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>Aida's Astounding Team vs. Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="L218" t="n">
+        <v>2</v>
+      </c>
+      <c r="M218" t="inlineStr">
+        <is>
+          <t>18Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="N218" t="n">
+        <v>6</v>
+      </c>
+      <c r="O218" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>18</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Away</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
         <v>46.94</v>
       </c>
-      <c r="F217" t="n">
+      <c r="F219" t="n">
         <v>46.94</v>
       </c>
-      <c r="G217" t="inlineStr">
+      <c r="G219" t="inlineStr">
         <is>
           <t>LOSERS_CONSOLATION_LADDER</t>
         </is>
       </c>
-      <c r="H217" t="n">
+      <c r="H219" t="n">
         <v>-58.12</v>
       </c>
-      <c r="I217" t="n">
+      <c r="I219" t="n">
         <v>-58.12</v>
       </c>
-      <c r="J217" t="inlineStr">
+      <c r="J219" t="inlineStr">
         <is>
           <t>Aida's Astounding Team vs. Kuppenheimer</t>
         </is>
       </c>
-      <c r="K217" t="inlineStr">
+      <c r="K219" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
       </c>
-      <c r="L217" t="n">
-        <v>1</v>
-      </c>
-      <c r="M217" t="inlineStr">
+      <c r="L219" t="n">
+        <v>1</v>
+      </c>
+      <c r="M219" t="inlineStr">
         <is>
           <t>18Kuppenheimer</t>
         </is>
       </c>
-      <c r="N217" t="n">
+      <c r="N219" t="n">
         <v>6</v>
       </c>
-      <c r="O217" t="n">
+      <c r="O219" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added final paragraph of box narrative, corrected matchup data which had 18 weeks
</commit_message>
<xml_diff>
--- a/matchups.xlsx
+++ b/matchups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F64458-FCD0-4F7C-959E-EF7503C4DB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4295F732-3C4D-4125-AE3F-004B3D2AD2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="336">
   <si>
     <t>Team</t>
   </si>
@@ -739,33 +739,6 @@
     <t>17Kuppenheimer</t>
   </si>
   <si>
-    <t>18Baby Back Gibbs</t>
-  </si>
-  <si>
-    <t>18Sith Happens</t>
-  </si>
-  <si>
-    <t>18Mighty Rubber Ducks</t>
-  </si>
-  <si>
-    <t>18Drafted by AI</t>
-  </si>
-  <si>
-    <t>18Compile and Conquer</t>
-  </si>
-  <si>
-    <t>18Apex Predators</t>
-  </si>
-  <si>
-    <t>18Boomer Sooners</t>
-  </si>
-  <si>
-    <t>18Bring the heat</t>
-  </si>
-  <si>
-    <t>18Kuppenheimer</t>
-  </si>
-  <si>
     <t>A's Astounding Team</t>
   </si>
   <si>
@@ -859,9 +832,6 @@
     <t>17A's Astounding Team</t>
   </si>
   <si>
-    <t>18A's Astounding Team</t>
-  </si>
-  <si>
     <t>K's Deluxe Team</t>
   </si>
   <si>
@@ -961,9 +931,6 @@
     <t>17K's Deluxe Team</t>
   </si>
   <si>
-    <t>18K's Deluxe Team</t>
-  </si>
-  <si>
     <t>Magic M</t>
   </si>
   <si>
@@ -1061,9 +1028,6 @@
   </si>
   <si>
     <t>17Magic M</t>
-  </si>
-  <si>
-    <t>18Magic M</t>
   </si>
 </sst>
 </file>
@@ -1426,9 +1390,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O219"/>
+  <dimension ref="A1:O207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1484,7 +1450,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1508,7 +1474,7 @@
         <v>-12.3</v>
       </c>
       <c r="J2" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
@@ -1528,7 +1494,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1555,7 +1521,7 @@
         <v>12.3</v>
       </c>
       <c r="J3" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
@@ -1564,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1669,7 +1635,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -1696,7 +1662,7 @@
         <v>9.44</v>
       </c>
       <c r="J6" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
@@ -1705,7 +1671,7 @@
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="N6">
         <v>3</v>
@@ -1719,7 +1685,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1743,7 +1709,7 @@
         <v>-9.44</v>
       </c>
       <c r="J7" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
@@ -1766,7 +1732,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1790,7 +1756,7 @@
         <v>-13.16</v>
       </c>
       <c r="J8" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="K8" t="s">
         <v>18</v>
@@ -1810,7 +1776,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -1837,7 +1803,7 @@
         <v>13.16</v>
       </c>
       <c r="J9" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="K9" t="s">
         <v>21</v>
@@ -1846,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="N9">
         <v>4</v>
@@ -2045,7 +2011,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -2072,7 +2038,7 @@
         <v>80.12</v>
       </c>
       <c r="J14" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="K14" t="s">
         <v>21</v>
@@ -2081,7 +2047,7 @@
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2095,7 +2061,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -2119,7 +2085,7 @@
         <v>-80.12</v>
       </c>
       <c r="J15" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="K15" t="s">
         <v>18</v>
@@ -2233,7 +2199,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -2260,7 +2226,7 @@
         <v>27.32</v>
       </c>
       <c r="J18" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="K18" t="s">
         <v>21</v>
@@ -2269,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="N18">
         <v>3</v>
@@ -2283,7 +2249,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -2307,7 +2273,7 @@
         <v>-27.32</v>
       </c>
       <c r="J19" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -2327,7 +2293,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
@@ -2354,7 +2320,7 @@
         <v>-47.92</v>
       </c>
       <c r="J20" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="K20" t="s">
         <v>18</v>
@@ -2363,7 +2329,7 @@
         <v>2</v>
       </c>
       <c r="M20" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="N20">
         <v>4</v>
@@ -2377,7 +2343,7 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -2401,7 +2367,7 @@
         <v>47.92</v>
       </c>
       <c r="J21" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="K21" t="s">
         <v>21</v>
@@ -2612,7 +2578,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -2636,7 +2602,7 @@
         <v>-3.36</v>
       </c>
       <c r="J26" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -2656,7 +2622,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -2683,7 +2649,7 @@
         <v>3.36</v>
       </c>
       <c r="J27" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="K27" t="s">
         <v>21</v>
@@ -2692,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -2706,7 +2672,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -2730,7 +2696,7 @@
         <v>-0.02</v>
       </c>
       <c r="J28" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="K28" t="s">
         <v>18</v>
@@ -2750,7 +2716,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
@@ -2777,7 +2743,7 @@
         <v>0.02</v>
       </c>
       <c r="J29" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="K29" t="s">
         <v>21</v>
@@ -2786,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -2894,7 +2860,7 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -2918,7 +2884,7 @@
         <v>87.26</v>
       </c>
       <c r="J32" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K32" t="s">
         <v>21</v>
@@ -2938,7 +2904,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
@@ -2965,7 +2931,7 @@
         <v>-87.26</v>
       </c>
       <c r="J33" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K33" t="s">
         <v>18</v>
@@ -2974,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="N33">
         <v>4</v>
@@ -3173,10 +3139,10 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B38" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -3200,7 +3166,7 @@
         <v>8.26</v>
       </c>
       <c r="J38" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="K38" t="s">
         <v>21</v>
@@ -3209,7 +3175,7 @@
         <v>2</v>
       </c>
       <c r="M38" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -3220,10 +3186,10 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B39" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C39">
         <v>4</v>
@@ -3247,7 +3213,7 @@
         <v>-8.26</v>
       </c>
       <c r="J39" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="K39" t="s">
         <v>18</v>
@@ -3256,7 +3222,7 @@
         <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -3455,7 +3421,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B44" t="s">
         <v>36</v>
@@ -3482,7 +3448,7 @@
         <v>-78.459999999999994</v>
       </c>
       <c r="J44" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="K44" t="s">
         <v>18</v>
@@ -3491,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="M44" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="N44">
         <v>4</v>
@@ -3505,7 +3471,7 @@
         <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C45">
         <v>4</v>
@@ -3529,7 +3495,7 @@
         <v>78.459999999999994</v>
       </c>
       <c r="J45" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="K45" t="s">
         <v>21</v>
@@ -3740,7 +3706,7 @@
         <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C50">
         <v>5</v>
@@ -3764,7 +3730,7 @@
         <v>54.08</v>
       </c>
       <c r="J50" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="K50" t="s">
         <v>21</v>
@@ -3784,7 +3750,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B51" t="s">
         <v>22</v>
@@ -3811,7 +3777,7 @@
         <v>-54.08</v>
       </c>
       <c r="J51" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="K51" t="s">
         <v>18</v>
@@ -3820,7 +3786,7 @@
         <v>1</v>
       </c>
       <c r="M51" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -3831,7 +3797,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
@@ -3858,7 +3824,7 @@
         <v>34.880000000000003</v>
       </c>
       <c r="J52" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="K52" t="s">
         <v>21</v>
@@ -3867,7 +3833,7 @@
         <v>2</v>
       </c>
       <c r="M52" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="N52">
         <v>2</v>
@@ -3881,7 +3847,7 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -3905,7 +3871,7 @@
         <v>-34.880000000000003</v>
       </c>
       <c r="J53" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="K53" t="s">
         <v>18</v>
@@ -4022,7 +3988,7 @@
         <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C56">
         <v>5</v>
@@ -4046,7 +4012,7 @@
         <v>34.700000000000003</v>
       </c>
       <c r="J56" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="K56" t="s">
         <v>21</v>
@@ -4066,7 +4032,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B57" t="s">
         <v>31</v>
@@ -4093,7 +4059,7 @@
         <v>-34.700000000000003</v>
       </c>
       <c r="J57" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="K57" t="s">
         <v>18</v>
@@ -4102,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="M57" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="N57">
         <v>4</v>
@@ -4301,10 +4267,10 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B62" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C62">
         <v>6</v>
@@ -4328,7 +4294,7 @@
         <v>45.26</v>
       </c>
       <c r="J62" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="K62" t="s">
         <v>21</v>
@@ -4337,7 +4303,7 @@
         <v>2</v>
       </c>
       <c r="M62" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -4348,10 +4314,10 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B63" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C63">
         <v>6</v>
@@ -4375,7 +4341,7 @@
         <v>-45.26</v>
       </c>
       <c r="J63" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="K63" t="s">
         <v>18</v>
@@ -4384,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="M63" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -4677,7 +4643,7 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B70" t="s">
         <v>36</v>
@@ -4704,7 +4670,7 @@
         <v>-31.48</v>
       </c>
       <c r="J70" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="K70" t="s">
         <v>18</v>
@@ -4713,7 +4679,7 @@
         <v>2</v>
       </c>
       <c r="M70" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="N70">
         <v>5</v>
@@ -4727,7 +4693,7 @@
         <v>36</v>
       </c>
       <c r="B71" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C71">
         <v>6</v>
@@ -4751,7 +4717,7 @@
         <v>31.48</v>
       </c>
       <c r="J71" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="K71" t="s">
         <v>21</v>
@@ -4865,7 +4831,7 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B74" t="s">
         <v>15</v>
@@ -4892,7 +4858,7 @@
         <v>23.62</v>
       </c>
       <c r="J74" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="K74" t="s">
         <v>21</v>
@@ -4901,7 +4867,7 @@
         <v>2</v>
       </c>
       <c r="M74" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="N74">
         <v>1</v>
@@ -4915,7 +4881,7 @@
         <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C75">
         <v>7</v>
@@ -4939,7 +4905,7 @@
         <v>-23.62</v>
       </c>
       <c r="J75" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="K75" t="s">
         <v>18</v>
@@ -5150,7 +5116,7 @@
         <v>37</v>
       </c>
       <c r="B80" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C80">
         <v>7</v>
@@ -5174,7 +5140,7 @@
         <v>32.56</v>
       </c>
       <c r="J80" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="K80" t="s">
         <v>21</v>
@@ -5194,7 +5160,7 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B81" t="s">
         <v>37</v>
@@ -5221,7 +5187,7 @@
         <v>-32.56</v>
       </c>
       <c r="J81" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="K81" t="s">
         <v>18</v>
@@ -5230,7 +5196,7 @@
         <v>1</v>
       </c>
       <c r="M81" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="N81">
         <v>4</v>
@@ -5338,7 +5304,7 @@
         <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C84">
         <v>7</v>
@@ -5362,7 +5328,7 @@
         <v>-18.64</v>
       </c>
       <c r="J84" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="K84" t="s">
         <v>18</v>
@@ -5382,7 +5348,7 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B85" t="s">
         <v>31</v>
@@ -5409,7 +5375,7 @@
         <v>18.64</v>
       </c>
       <c r="J85" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="K85" t="s">
         <v>21</v>
@@ -5418,7 +5384,7 @@
         <v>1</v>
       </c>
       <c r="M85" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="N85">
         <v>6</v>
@@ -5432,7 +5398,7 @@
         <v>23</v>
       </c>
       <c r="B86" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C86">
         <v>8</v>
@@ -5456,7 +5422,7 @@
         <v>-6.98</v>
       </c>
       <c r="J86" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="K86" t="s">
         <v>18</v>
@@ -5476,7 +5442,7 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B87" t="s">
         <v>23</v>
@@ -5503,7 +5469,7 @@
         <v>6.98</v>
       </c>
       <c r="J87" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="K87" t="s">
         <v>21</v>
@@ -5512,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="M87" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="N87">
         <v>1</v>
@@ -5617,7 +5583,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B90" t="s">
         <v>32</v>
@@ -5644,7 +5610,7 @@
         <v>14.16</v>
       </c>
       <c r="J90" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="K90" t="s">
         <v>21</v>
@@ -5653,7 +5619,7 @@
         <v>2</v>
       </c>
       <c r="M90" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="N90">
         <v>3</v>
@@ -5667,7 +5633,7 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C91">
         <v>8</v>
@@ -5691,7 +5657,7 @@
         <v>-14.16</v>
       </c>
       <c r="J91" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="K91" t="s">
         <v>18</v>
@@ -5805,7 +5771,7 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B94" t="s">
         <v>36</v>
@@ -5832,7 +5798,7 @@
         <v>-67.52</v>
       </c>
       <c r="J94" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="K94" t="s">
         <v>18</v>
@@ -5841,7 +5807,7 @@
         <v>2</v>
       </c>
       <c r="M94" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="N94">
         <v>5</v>
@@ -5855,7 +5821,7 @@
         <v>36</v>
       </c>
       <c r="B95" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C95">
         <v>8</v>
@@ -5879,7 +5845,7 @@
         <v>67.52</v>
       </c>
       <c r="J95" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="K95" t="s">
         <v>21</v>
@@ -5993,7 +5959,7 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B98" t="s">
         <v>27</v>
@@ -6020,7 +5986,7 @@
         <v>21.6</v>
       </c>
       <c r="J98" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="K98" t="s">
         <v>21</v>
@@ -6029,7 +5995,7 @@
         <v>2</v>
       </c>
       <c r="M98" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="N98">
         <v>1</v>
@@ -6043,7 +6009,7 @@
         <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C99">
         <v>9</v>
@@ -6067,7 +6033,7 @@
         <v>-21.6</v>
       </c>
       <c r="J99" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="K99" t="s">
         <v>18</v>
@@ -6090,7 +6056,7 @@
         <v>29</v>
       </c>
       <c r="B100" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C100">
         <v>9</v>
@@ -6114,7 +6080,7 @@
         <v>-11.12</v>
       </c>
       <c r="J100" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="K100" t="s">
         <v>18</v>
@@ -6134,7 +6100,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B101" t="s">
         <v>29</v>
@@ -6161,7 +6127,7 @@
         <v>11.12</v>
       </c>
       <c r="J101" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="K101" t="s">
         <v>21</v>
@@ -6170,7 +6136,7 @@
         <v>1</v>
       </c>
       <c r="M101" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="N101">
         <v>2</v>
@@ -6278,7 +6244,7 @@
         <v>37</v>
       </c>
       <c r="B104" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C104">
         <v>9</v>
@@ -6302,7 +6268,7 @@
         <v>30.08</v>
       </c>
       <c r="J104" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="K104" t="s">
         <v>21</v>
@@ -6322,7 +6288,7 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B105" t="s">
         <v>37</v>
@@ -6349,7 +6315,7 @@
         <v>-30.08</v>
       </c>
       <c r="J105" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="K105" t="s">
         <v>18</v>
@@ -6358,7 +6324,7 @@
         <v>1</v>
       </c>
       <c r="M105" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="N105">
         <v>4</v>
@@ -6557,10 +6523,10 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B110" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C110">
         <v>10</v>
@@ -6584,7 +6550,7 @@
         <v>23.8</v>
       </c>
       <c r="J110" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="K110" t="s">
         <v>21</v>
@@ -6593,7 +6559,7 @@
         <v>2</v>
       </c>
       <c r="M110" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="N110">
         <v>1</v>
@@ -6604,10 +6570,10 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B111" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C111">
         <v>10</v>
@@ -6631,7 +6597,7 @@
         <v>-23.8</v>
       </c>
       <c r="J111" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="K111" t="s">
         <v>18</v>
@@ -6640,7 +6606,7 @@
         <v>1</v>
       </c>
       <c r="M111" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="N111">
         <v>1</v>
@@ -6745,7 +6711,7 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B114" t="s">
         <v>32</v>
@@ -6772,7 +6738,7 @@
         <v>-32.380000000000003</v>
       </c>
       <c r="J114" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="K114" t="s">
         <v>18</v>
@@ -6781,7 +6747,7 @@
         <v>2</v>
       </c>
       <c r="M114" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="N114">
         <v>3</v>
@@ -6795,7 +6761,7 @@
         <v>32</v>
       </c>
       <c r="B115" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C115">
         <v>10</v>
@@ -6819,7 +6785,7 @@
         <v>32.380000000000003</v>
       </c>
       <c r="J115" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="K115" t="s">
         <v>21</v>
@@ -7121,7 +7087,7 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B122" t="s">
         <v>22</v>
@@ -7148,7 +7114,7 @@
         <v>102.26</v>
       </c>
       <c r="J122" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="K122" t="s">
         <v>21</v>
@@ -7157,7 +7123,7 @@
         <v>2</v>
       </c>
       <c r="M122" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="N122">
         <v>1</v>
@@ -7171,7 +7137,7 @@
         <v>22</v>
       </c>
       <c r="B123" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C123">
         <v>11</v>
@@ -7195,7 +7161,7 @@
         <v>-102.26</v>
       </c>
       <c r="J123" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="K123" t="s">
         <v>18</v>
@@ -7218,7 +7184,7 @@
         <v>29</v>
       </c>
       <c r="B124" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C124">
         <v>11</v>
@@ -7242,7 +7208,7 @@
         <v>67.3</v>
       </c>
       <c r="J124" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="K124" t="s">
         <v>21</v>
@@ -7262,7 +7228,7 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B125" t="s">
         <v>29</v>
@@ -7289,7 +7255,7 @@
         <v>-67.3</v>
       </c>
       <c r="J125" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="K125" t="s">
         <v>18</v>
@@ -7298,7 +7264,7 @@
         <v>1</v>
       </c>
       <c r="M125" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="N125">
         <v>2</v>
@@ -7594,7 +7560,7 @@
         <v>31</v>
       </c>
       <c r="B132" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C132">
         <v>11</v>
@@ -7618,7 +7584,7 @@
         <v>-43.24</v>
       </c>
       <c r="J132" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="K132" t="s">
         <v>18</v>
@@ -7638,7 +7604,7 @@
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B133" t="s">
         <v>31</v>
@@ -7665,7 +7631,7 @@
         <v>43.24</v>
       </c>
       <c r="J133" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="K133" t="s">
         <v>21</v>
@@ -7674,7 +7640,7 @@
         <v>1</v>
       </c>
       <c r="M133" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="N133">
         <v>6</v>
@@ -7685,10 +7651,10 @@
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B134" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C134">
         <v>12</v>
@@ -7712,7 +7678,7 @@
         <v>45.66</v>
       </c>
       <c r="J134" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="K134" t="s">
         <v>21</v>
@@ -7721,7 +7687,7 @@
         <v>2</v>
       </c>
       <c r="M134" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="N134">
         <v>1</v>
@@ -7732,10 +7698,10 @@
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C135">
         <v>12</v>
@@ -7759,7 +7725,7 @@
         <v>-45.66</v>
       </c>
       <c r="J135" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="K135" t="s">
         <v>18</v>
@@ -7768,7 +7734,7 @@
         <v>1</v>
       </c>
       <c r="M135" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="N135">
         <v>1</v>
@@ -8064,7 +8030,7 @@
         <v>36</v>
       </c>
       <c r="B142" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C142">
         <v>12</v>
@@ -8088,7 +8054,7 @@
         <v>28.9</v>
       </c>
       <c r="J142" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="K142" t="s">
         <v>21</v>
@@ -8108,7 +8074,7 @@
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B143" t="s">
         <v>36</v>
@@ -8135,7 +8101,7 @@
         <v>-28.9</v>
       </c>
       <c r="J143" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="K143" t="s">
         <v>18</v>
@@ -8144,7 +8110,7 @@
         <v>1</v>
       </c>
       <c r="M143" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="N143">
         <v>5</v>
@@ -8252,7 +8218,7 @@
         <v>15</v>
       </c>
       <c r="B146" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C146">
         <v>13</v>
@@ -8276,7 +8242,7 @@
         <v>-65.62</v>
       </c>
       <c r="J146" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="K146" t="s">
         <v>18</v>
@@ -8296,7 +8262,7 @@
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B147" t="s">
         <v>15</v>
@@ -8323,7 +8289,7 @@
         <v>65.62</v>
       </c>
       <c r="J147" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="K147" t="s">
         <v>21</v>
@@ -8332,7 +8298,7 @@
         <v>1</v>
       </c>
       <c r="M147" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="N147">
         <v>1</v>
@@ -8531,7 +8497,7 @@
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B152" t="s">
         <v>37</v>
@@ -8558,7 +8524,7 @@
         <v>15.52</v>
       </c>
       <c r="J152" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="K152" t="s">
         <v>21</v>
@@ -8567,7 +8533,7 @@
         <v>2</v>
       </c>
       <c r="M152" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="N152">
         <v>4</v>
@@ -8581,7 +8547,7 @@
         <v>37</v>
       </c>
       <c r="B153" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C153">
         <v>13</v>
@@ -8605,7 +8571,7 @@
         <v>-15.52</v>
       </c>
       <c r="J153" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="K153" t="s">
         <v>18</v>
@@ -8719,7 +8685,7 @@
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B156" t="s">
         <v>31</v>
@@ -8746,7 +8712,7 @@
         <v>-6.32</v>
       </c>
       <c r="J156" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="K156" t="s">
         <v>18</v>
@@ -8755,7 +8721,7 @@
         <v>2</v>
       </c>
       <c r="M156" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="N156">
         <v>6</v>
@@ -8769,7 +8735,7 @@
         <v>31</v>
       </c>
       <c r="B157" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C157">
         <v>13</v>
@@ -8793,7 +8759,7 @@
         <v>6.32</v>
       </c>
       <c r="J157" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="K157" t="s">
         <v>21</v>
@@ -8813,7 +8779,7 @@
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B158" t="s">
         <v>23</v>
@@ -8840,7 +8806,7 @@
         <v>-24.8</v>
       </c>
       <c r="J158" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="K158" t="s">
         <v>18</v>
@@ -8849,7 +8815,7 @@
         <v>2</v>
       </c>
       <c r="M158" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="N158">
         <v>1</v>
@@ -8863,7 +8829,7 @@
         <v>23</v>
       </c>
       <c r="B159" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C159">
         <v>14</v>
@@ -8887,7 +8853,7 @@
         <v>24.8</v>
       </c>
       <c r="J159" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="K159" t="s">
         <v>21</v>
@@ -9004,7 +8970,7 @@
         <v>32</v>
       </c>
       <c r="B162" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C162">
         <v>14</v>
@@ -9028,7 +8994,7 @@
         <v>-19.02</v>
       </c>
       <c r="J162" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="K162" t="s">
         <v>18</v>
@@ -9048,7 +9014,7 @@
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B163" t="s">
         <v>32</v>
@@ -9075,7 +9041,7 @@
         <v>19.02</v>
       </c>
       <c r="J163" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="K163" t="s">
         <v>21</v>
@@ -9084,7 +9050,7 @@
         <v>1</v>
       </c>
       <c r="M163" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="N163">
         <v>3</v>
@@ -9192,7 +9158,7 @@
         <v>36</v>
       </c>
       <c r="B166" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C166">
         <v>14</v>
@@ -9216,7 +9182,7 @@
         <v>91.48</v>
       </c>
       <c r="J166" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="K166" t="s">
         <v>21</v>
@@ -9236,7 +9202,7 @@
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B167" t="s">
         <v>36</v>
@@ -9263,7 +9229,7 @@
         <v>-91.48</v>
       </c>
       <c r="J167" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="K167" t="s">
         <v>18</v>
@@ -9272,7 +9238,7 @@
         <v>1</v>
       </c>
       <c r="M167" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="N167">
         <v>5</v>
@@ -9659,7 +9625,7 @@
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B176" t="s">
         <v>201</v>
@@ -9686,7 +9652,7 @@
         <v>122.16</v>
       </c>
       <c r="J176" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="K176" t="s">
         <v>21</v>
@@ -9695,7 +9661,7 @@
         <v>2</v>
       </c>
       <c r="M176" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="N176">
         <v>4</v>
@@ -9709,7 +9675,7 @@
         <v>201</v>
       </c>
       <c r="B177" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C177">
         <v>15</v>
@@ -9733,7 +9699,7 @@
         <v>-122.16</v>
       </c>
       <c r="J177" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="K177" t="s">
         <v>18</v>
@@ -9756,7 +9722,7 @@
         <v>32</v>
       </c>
       <c r="B178" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C178">
         <v>15</v>
@@ -9780,7 +9746,7 @@
         <v>20.68</v>
       </c>
       <c r="J178" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="K178" t="s">
         <v>21</v>
@@ -9800,7 +9766,7 @@
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B179" t="s">
         <v>32</v>
@@ -9827,7 +9793,7 @@
         <v>-20.68</v>
       </c>
       <c r="J179" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="K179" t="s">
         <v>18</v>
@@ -9836,7 +9802,7 @@
         <v>1</v>
       </c>
       <c r="M179" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="N179">
         <v>5</v>
@@ -9847,7 +9813,7 @@
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B180" t="s">
         <v>37</v>
@@ -9874,7 +9840,7 @@
         <v>-12.02</v>
       </c>
       <c r="J180" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="K180" t="s">
         <v>18</v>
@@ -9883,7 +9849,7 @@
         <v>2</v>
       </c>
       <c r="M180" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="N180">
         <v>6</v>
@@ -9897,7 +9863,7 @@
         <v>37</v>
       </c>
       <c r="B181" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C181">
         <v>15</v>
@@ -9921,7 +9887,7 @@
         <v>12.02</v>
       </c>
       <c r="J181" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="K181" t="s">
         <v>21</v>
@@ -10129,7 +10095,7 @@
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B186" t="s">
         <v>22</v>
@@ -10156,7 +10122,7 @@
         <v>35.5</v>
       </c>
       <c r="J186" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="K186" t="s">
         <v>21</v>
@@ -10165,7 +10131,7 @@
         <v>2</v>
       </c>
       <c r="M186" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="N186">
         <v>2</v>
@@ -10179,7 +10145,7 @@
         <v>22</v>
       </c>
       <c r="B187" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C187">
         <v>16</v>
@@ -10203,7 +10169,7 @@
         <v>-35.5</v>
       </c>
       <c r="J187" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="K187" t="s">
         <v>18</v>
@@ -10411,7 +10377,7 @@
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B192" t="s">
         <v>29</v>
@@ -10438,7 +10404,7 @@
         <v>-34.659999999999997</v>
       </c>
       <c r="J192" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="K192" t="s">
         <v>18</v>
@@ -10447,7 +10413,7 @@
         <v>2</v>
       </c>
       <c r="M192" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="N192">
         <v>5</v>
@@ -10461,7 +10427,7 @@
         <v>29</v>
       </c>
       <c r="B193" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C193">
         <v>16</v>
@@ -10485,7 +10451,7 @@
         <v>34.659999999999997</v>
       </c>
       <c r="J193" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="K193" t="s">
         <v>21</v>
@@ -10505,7 +10471,7 @@
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B194" t="s">
         <v>15</v>
@@ -10532,7 +10498,7 @@
         <v>32.28</v>
       </c>
       <c r="J194" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="K194" t="s">
         <v>21</v>
@@ -10541,7 +10507,7 @@
         <v>2</v>
       </c>
       <c r="M194" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="N194">
         <v>6</v>
@@ -10555,7 +10521,7 @@
         <v>15</v>
       </c>
       <c r="B195" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C195">
         <v>16</v>
@@ -10579,7 +10545,7 @@
         <v>-32.28</v>
       </c>
       <c r="J195" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="K195" t="s">
         <v>18</v>
@@ -10602,7 +10568,7 @@
         <v>36</v>
       </c>
       <c r="B196" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C196">
         <v>17</v>
@@ -10626,7 +10592,7 @@
         <v>29.04</v>
       </c>
       <c r="J196" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="K196" t="s">
         <v>21</v>
@@ -10646,7 +10612,7 @@
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B197" t="s">
         <v>36</v>
@@ -10673,7 +10639,7 @@
         <v>-29.04</v>
       </c>
       <c r="J197" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="K197" t="s">
         <v>18</v>
@@ -10682,7 +10648,7 @@
         <v>1</v>
       </c>
       <c r="M197" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="N197">
         <v>1</v>
@@ -10975,7 +10941,7 @@
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B204" t="s">
         <v>37</v>
@@ -11002,7 +10968,7 @@
         <v>-33.18</v>
       </c>
       <c r="J204" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="K204" t="s">
         <v>18</v>
@@ -11011,7 +10977,7 @@
         <v>2</v>
       </c>
       <c r="M204" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="N204">
         <v>5</v>
@@ -11025,7 +10991,7 @@
         <v>37</v>
       </c>
       <c r="B205" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C205">
         <v>17</v>
@@ -11049,7 +11015,7 @@
         <v>33.18</v>
       </c>
       <c r="J205" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="K205" t="s">
         <v>21</v>
@@ -11069,7 +11035,7 @@
     </row>
     <row r="206" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B206" t="s">
         <v>15</v>
@@ -11096,7 +11062,7 @@
         <v>58.12</v>
       </c>
       <c r="J206" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="K206" t="s">
         <v>21</v>
@@ -11105,7 +11071,7 @@
         <v>2</v>
       </c>
       <c r="M206" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="N206">
         <v>6</v>
@@ -11119,7 +11085,7 @@
         <v>15</v>
       </c>
       <c r="B207" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C207">
         <v>17</v>
@@ -11143,7 +11109,7 @@
         <v>-58.12</v>
       </c>
       <c r="J207" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="K207" t="s">
         <v>18</v>
@@ -11158,570 +11124,6 @@
         <v>6</v>
       </c>
       <c r="O207">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
-        <v>36</v>
-      </c>
-      <c r="B208" t="s">
-        <v>314</v>
-      </c>
-      <c r="C208">
-        <v>18</v>
-      </c>
-      <c r="D208" t="s">
-        <v>16</v>
-      </c>
-      <c r="E208">
-        <v>159.36000000000001</v>
-      </c>
-      <c r="F208">
-        <v>159.36000000000001</v>
-      </c>
-      <c r="G208" t="s">
-        <v>202</v>
-      </c>
-      <c r="H208">
-        <v>29.04</v>
-      </c>
-      <c r="I208">
-        <v>29.04</v>
-      </c>
-      <c r="J208" t="s">
-        <v>337</v>
-      </c>
-      <c r="K208" t="s">
-        <v>21</v>
-      </c>
-      <c r="L208">
-        <v>2</v>
-      </c>
-      <c r="M208" t="s">
-        <v>239</v>
-      </c>
-      <c r="N208">
-        <v>1</v>
-      </c>
-      <c r="O208">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A209" t="s">
-        <v>314</v>
-      </c>
-      <c r="B209" t="s">
-        <v>36</v>
-      </c>
-      <c r="C209">
-        <v>18</v>
-      </c>
-      <c r="D209" t="s">
-        <v>20</v>
-      </c>
-      <c r="E209">
-        <v>130.32</v>
-      </c>
-      <c r="F209">
-        <v>130.32</v>
-      </c>
-      <c r="G209" t="s">
-        <v>202</v>
-      </c>
-      <c r="H209">
-        <v>-29.04</v>
-      </c>
-      <c r="I209">
-        <v>-29.04</v>
-      </c>
-      <c r="J209" t="s">
-        <v>337</v>
-      </c>
-      <c r="K209" t="s">
-        <v>18</v>
-      </c>
-      <c r="L209">
-        <v>1</v>
-      </c>
-      <c r="M209" t="s">
-        <v>347</v>
-      </c>
-      <c r="N209">
-        <v>1</v>
-      </c>
-      <c r="O209">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A210" t="s">
-        <v>22</v>
-      </c>
-      <c r="B210" t="s">
-        <v>23</v>
-      </c>
-      <c r="C210">
-        <v>18</v>
-      </c>
-      <c r="D210" t="s">
-        <v>16</v>
-      </c>
-      <c r="E210">
-        <v>140.88</v>
-      </c>
-      <c r="F210">
-        <v>140.88</v>
-      </c>
-      <c r="G210" t="s">
-        <v>221</v>
-      </c>
-      <c r="H210">
-        <v>67.180000000000007</v>
-      </c>
-      <c r="I210">
-        <v>67.180000000000007</v>
-      </c>
-      <c r="J210" t="s">
-        <v>24</v>
-      </c>
-      <c r="K210" t="s">
-        <v>21</v>
-      </c>
-      <c r="L210">
-        <v>2</v>
-      </c>
-      <c r="M210" t="s">
-        <v>240</v>
-      </c>
-      <c r="N210">
-        <v>2</v>
-      </c>
-      <c r="O210">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A211" t="s">
-        <v>23</v>
-      </c>
-      <c r="B211" t="s">
-        <v>22</v>
-      </c>
-      <c r="C211">
-        <v>18</v>
-      </c>
-      <c r="D211" t="s">
-        <v>20</v>
-      </c>
-      <c r="E211">
-        <v>73.7</v>
-      </c>
-      <c r="F211">
-        <v>73.7</v>
-      </c>
-      <c r="G211" t="s">
-        <v>221</v>
-      </c>
-      <c r="H211">
-        <v>-67.180000000000007</v>
-      </c>
-      <c r="I211">
-        <v>-67.180000000000007</v>
-      </c>
-      <c r="J211" t="s">
-        <v>24</v>
-      </c>
-      <c r="K211" t="s">
-        <v>18</v>
-      </c>
-      <c r="L211">
-        <v>1</v>
-      </c>
-      <c r="M211" t="s">
-        <v>241</v>
-      </c>
-      <c r="N211">
-        <v>2</v>
-      </c>
-      <c r="O211">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A212" t="s">
-        <v>27</v>
-      </c>
-      <c r="B212" t="s">
-        <v>31</v>
-      </c>
-      <c r="C212">
-        <v>18</v>
-      </c>
-      <c r="D212" t="s">
-        <v>16</v>
-      </c>
-      <c r="E212">
-        <v>134.47999999999999</v>
-      </c>
-      <c r="F212">
-        <v>134.47999999999999</v>
-      </c>
-      <c r="G212" t="s">
-        <v>221</v>
-      </c>
-      <c r="H212">
-        <v>-20.8</v>
-      </c>
-      <c r="I212">
-        <v>-20.8</v>
-      </c>
-      <c r="J212" t="s">
-        <v>149</v>
-      </c>
-      <c r="K212" t="s">
-        <v>18</v>
-      </c>
-      <c r="L212">
-        <v>2</v>
-      </c>
-      <c r="M212" t="s">
-        <v>242</v>
-      </c>
-      <c r="N212">
-        <v>3</v>
-      </c>
-      <c r="O212">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A213" t="s">
-        <v>31</v>
-      </c>
-      <c r="B213" t="s">
-        <v>27</v>
-      </c>
-      <c r="C213">
-        <v>18</v>
-      </c>
-      <c r="D213" t="s">
-        <v>20</v>
-      </c>
-      <c r="E213">
-        <v>155.28</v>
-      </c>
-      <c r="F213">
-        <v>155.28</v>
-      </c>
-      <c r="G213" t="s">
-        <v>221</v>
-      </c>
-      <c r="H213">
-        <v>20.8</v>
-      </c>
-      <c r="I213">
-        <v>20.8</v>
-      </c>
-      <c r="J213" t="s">
-        <v>149</v>
-      </c>
-      <c r="K213" t="s">
-        <v>21</v>
-      </c>
-      <c r="L213">
-        <v>1</v>
-      </c>
-      <c r="M213" t="s">
-        <v>243</v>
-      </c>
-      <c r="N213">
-        <v>3</v>
-      </c>
-      <c r="O213">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A214" t="s">
-        <v>32</v>
-      </c>
-      <c r="B214" t="s">
-        <v>29</v>
-      </c>
-      <c r="C214">
-        <v>18</v>
-      </c>
-      <c r="D214" t="s">
-        <v>16</v>
-      </c>
-      <c r="E214">
-        <v>158.88</v>
-      </c>
-      <c r="F214">
-        <v>158.88</v>
-      </c>
-      <c r="G214" t="s">
-        <v>212</v>
-      </c>
-      <c r="H214">
-        <v>72.400000000000006</v>
-      </c>
-      <c r="I214">
-        <v>72.400000000000006</v>
-      </c>
-      <c r="J214" t="s">
-        <v>234</v>
-      </c>
-      <c r="K214" t="s">
-        <v>21</v>
-      </c>
-      <c r="L214">
-        <v>2</v>
-      </c>
-      <c r="M214" t="s">
-        <v>244</v>
-      </c>
-      <c r="N214">
-        <v>4</v>
-      </c>
-      <c r="O214">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A215" t="s">
-        <v>29</v>
-      </c>
-      <c r="B215" t="s">
-        <v>32</v>
-      </c>
-      <c r="C215">
-        <v>18</v>
-      </c>
-      <c r="D215" t="s">
-        <v>20</v>
-      </c>
-      <c r="E215">
-        <v>86.48</v>
-      </c>
-      <c r="F215">
-        <v>86.48</v>
-      </c>
-      <c r="G215" t="s">
-        <v>212</v>
-      </c>
-      <c r="H215">
-        <v>-72.400000000000006</v>
-      </c>
-      <c r="I215">
-        <v>-72.400000000000006</v>
-      </c>
-      <c r="J215" t="s">
-        <v>234</v>
-      </c>
-      <c r="K215" t="s">
-        <v>18</v>
-      </c>
-      <c r="L215">
-        <v>1</v>
-      </c>
-      <c r="M215" t="s">
-        <v>245</v>
-      </c>
-      <c r="N215">
-        <v>4</v>
-      </c>
-      <c r="O215">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A216" t="s">
-        <v>280</v>
-      </c>
-      <c r="B216" t="s">
-        <v>37</v>
-      </c>
-      <c r="C216">
-        <v>18</v>
-      </c>
-      <c r="D216" t="s">
-        <v>16</v>
-      </c>
-      <c r="E216">
-        <v>75.7</v>
-      </c>
-      <c r="F216">
-        <v>75.7</v>
-      </c>
-      <c r="G216" t="s">
-        <v>212</v>
-      </c>
-      <c r="H216">
-        <v>-33.18</v>
-      </c>
-      <c r="I216">
-        <v>-33.18</v>
-      </c>
-      <c r="J216" t="s">
-        <v>308</v>
-      </c>
-      <c r="K216" t="s">
-        <v>18</v>
-      </c>
-      <c r="L216">
-        <v>2</v>
-      </c>
-      <c r="M216" t="s">
-        <v>313</v>
-      </c>
-      <c r="N216">
-        <v>5</v>
-      </c>
-      <c r="O216">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A217" t="s">
-        <v>37</v>
-      </c>
-      <c r="B217" t="s">
-        <v>280</v>
-      </c>
-      <c r="C217">
-        <v>18</v>
-      </c>
-      <c r="D217" t="s">
-        <v>20</v>
-      </c>
-      <c r="E217">
-        <v>108.88</v>
-      </c>
-      <c r="F217">
-        <v>108.88</v>
-      </c>
-      <c r="G217" t="s">
-        <v>212</v>
-      </c>
-      <c r="H217">
-        <v>33.18</v>
-      </c>
-      <c r="I217">
-        <v>33.18</v>
-      </c>
-      <c r="J217" t="s">
-        <v>308</v>
-      </c>
-      <c r="K217" t="s">
-        <v>21</v>
-      </c>
-      <c r="L217">
-        <v>1</v>
-      </c>
-      <c r="M217" t="s">
-        <v>246</v>
-      </c>
-      <c r="N217">
-        <v>5</v>
-      </c>
-      <c r="O217">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
-        <v>248</v>
-      </c>
-      <c r="B218" t="s">
-        <v>15</v>
-      </c>
-      <c r="C218">
-        <v>18</v>
-      </c>
-      <c r="D218" t="s">
-        <v>16</v>
-      </c>
-      <c r="E218">
-        <v>105.06</v>
-      </c>
-      <c r="F218">
-        <v>105.06</v>
-      </c>
-      <c r="G218" t="s">
-        <v>212</v>
-      </c>
-      <c r="H218">
-        <v>58.12</v>
-      </c>
-      <c r="I218">
-        <v>58.12</v>
-      </c>
-      <c r="J218" t="s">
-        <v>260</v>
-      </c>
-      <c r="K218" t="s">
-        <v>21</v>
-      </c>
-      <c r="L218">
-        <v>2</v>
-      </c>
-      <c r="M218" t="s">
-        <v>279</v>
-      </c>
-      <c r="N218">
-        <v>6</v>
-      </c>
-      <c r="O218">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A219" t="s">
-        <v>15</v>
-      </c>
-      <c r="B219" t="s">
-        <v>248</v>
-      </c>
-      <c r="C219">
-        <v>18</v>
-      </c>
-      <c r="D219" t="s">
-        <v>20</v>
-      </c>
-      <c r="E219">
-        <v>46.94</v>
-      </c>
-      <c r="F219">
-        <v>46.94</v>
-      </c>
-      <c r="G219" t="s">
-        <v>212</v>
-      </c>
-      <c r="H219">
-        <v>-58.12</v>
-      </c>
-      <c r="I219">
-        <v>-58.12</v>
-      </c>
-      <c r="J219" t="s">
-        <v>260</v>
-      </c>
-      <c r="K219" t="s">
-        <v>18</v>
-      </c>
-      <c r="L219">
-        <v>1</v>
-      </c>
-      <c r="M219" t="s">
-        <v>247</v>
-      </c>
-      <c r="N219">
-        <v>6</v>
-      </c>
-      <c r="O219">
         <v>6</v>
       </c>
     </row>

</xml_diff>